<commit_message>
add discipline data and output
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11DDCB49-53BF-0249-990B-1DD39F3D73FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8937309-326F-3D4D-A7C9-DA7D5FB57002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2540" windowWidth="27240" windowHeight="16440" xr2:uid="{1F989F6B-AFCF-AF42-9D0E-3D35A3A081C6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>21st Century Preparatory School</t>
   </si>
@@ -229,14 +229,21 @@
   </si>
   <si>
     <t>PPIN</t>
+  </si>
+  <si>
+    <t>NCES</t>
+  </si>
+  <si>
+    <t>District Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0000"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -307,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -321,6 +328,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,21 +648,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C62E933-5DF9-6143-AEAA-89AA45FFA9EF}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="30.5" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
@@ -669,14 +683,20 @@
         <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,12 +713,18 @@
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="5">
+      <c r="G2">
+        <v>8110</v>
+      </c>
+      <c r="H2" s="5">
         <v>100</v>
       </c>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="9">
+        <v>550004502575</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -713,12 +739,18 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3">
+        <v>4620</v>
+      </c>
+      <c r="H3" s="6">
         <v>491</v>
       </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="9">
+        <v>551236001621</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -733,12 +765,15 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
+        <v>4620</v>
+      </c>
+      <c r="H4" s="5">
         <v>1698</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -755,12 +790,15 @@
         <v>1</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="5">
+      <c r="G5">
+        <v>4620</v>
+      </c>
+      <c r="H5" s="5">
         <v>441</v>
       </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -777,15 +815,18 @@
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="5">
+      <c r="G6">
+        <v>4620</v>
+      </c>
+      <c r="H6" s="5">
         <v>1681</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,12 +841,18 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="5">
+      <c r="G7">
+        <v>4620</v>
+      </c>
+      <c r="H7" s="5">
         <v>118</v>
       </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="9">
+        <v>551236001611</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -820,12 +867,18 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="5">
+      <c r="G8">
+        <v>4620</v>
+      </c>
+      <c r="H8" s="5">
         <v>121</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="9">
+        <v>551236001614</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -842,12 +895,18 @@
         <v>1</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="5">
+      <c r="G9">
+        <v>4620</v>
+      </c>
+      <c r="H9" s="5">
         <v>119</v>
       </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="9">
+        <v>551236002311</v>
+      </c>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -864,12 +923,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="5">
+      <c r="G10">
+        <v>4620</v>
+      </c>
+      <c r="H10" s="5">
         <v>106</v>
       </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="9">
+        <v>551236001608</v>
+      </c>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -884,12 +949,15 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="5">
+      <c r="G11">
+        <v>4620</v>
+      </c>
+      <c r="H11" s="5">
         <v>122</v>
       </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -906,15 +974,18 @@
         <v>1</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="5">
+      <c r="G12">
+        <v>4620</v>
+      </c>
+      <c r="H12" s="5">
         <v>1711</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -929,12 +1000,15 @@
       <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13">
+        <v>4620</v>
+      </c>
+      <c r="H13" s="5">
         <v>492</v>
       </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -949,12 +1023,18 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="5">
+      <c r="G14">
+        <v>4620</v>
+      </c>
+      <c r="H14" s="5">
         <v>130</v>
       </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="9">
+        <v>551236001622</v>
+      </c>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -969,12 +1049,18 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="5">
+      <c r="G15">
+        <v>4620</v>
+      </c>
+      <c r="H15" s="5">
         <v>132</v>
       </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="9">
+        <v>551236001623</v>
+      </c>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -991,12 +1077,18 @@
         <v>1</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="5">
+      <c r="G16">
+        <v>4620</v>
+      </c>
+      <c r="H16" s="5">
         <v>314</v>
       </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="9">
+        <v>551236001624</v>
+      </c>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1013,12 +1105,13 @@
         <v>1</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="H17">
+      <c r="G17"/>
+      <c r="I17">
         <v>1507085</v>
       </c>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1033,12 +1126,18 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="5">
+      <c r="G18">
+        <v>4620</v>
+      </c>
+      <c r="H18" s="5">
         <v>136</v>
       </c>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="9">
+        <v>551236001626</v>
+      </c>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1053,12 +1152,18 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="5">
+      <c r="G19">
+        <v>4620</v>
+      </c>
+      <c r="H19" s="5">
         <v>111</v>
       </c>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="9">
+        <v>551236001627</v>
+      </c>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1073,12 +1178,18 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="5">
+      <c r="G20">
+        <v>4620</v>
+      </c>
+      <c r="H20" s="5">
         <v>720</v>
       </c>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="9">
+        <v>551236003337</v>
+      </c>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1093,12 +1204,18 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="5">
+      <c r="G21">
+        <v>4620</v>
+      </c>
+      <c r="H21" s="5">
         <v>138</v>
       </c>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="9">
+        <v>551236001628</v>
+      </c>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1113,15 +1230,18 @@
       <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22">
+        <v>4620</v>
+      </c>
+      <c r="H22" s="5">
         <v>2370</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>1512696</v>
       </c>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1138,12 +1258,18 @@
         <v>1</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="5">
+      <c r="G23">
+        <v>4620</v>
+      </c>
+      <c r="H23" s="5">
         <v>148</v>
       </c>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="9">
+        <v>551236001632</v>
+      </c>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1158,12 +1284,18 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="5">
+      <c r="G24">
+        <v>4620</v>
+      </c>
+      <c r="H24" s="5">
         <v>150</v>
       </c>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="9">
+        <v>551236001634</v>
+      </c>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1178,12 +1310,18 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="5">
+      <c r="G25">
+        <v>4620</v>
+      </c>
+      <c r="H25" s="5">
         <v>112</v>
       </c>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="9">
+        <v>551236001605</v>
+      </c>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1200,12 +1338,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="H26" t="s">
+      <c r="G26"/>
+      <c r="I26" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1220,12 +1359,18 @@
       <c r="F27" s="2">
         <v>1</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27">
+        <v>4620</v>
+      </c>
+      <c r="H27" s="5">
         <v>494</v>
       </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="9">
+        <v>551236001635</v>
+      </c>
+      <c r="N27" s="7"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1240,9 +1385,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G28"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1257,9 +1403,10 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G29"/>
+      <c r="N29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1274,9 +1421,10 @@
       <c r="F30" s="2">
         <v>1</v>
       </c>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G30"/>
+      <c r="N30" s="7"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1295,9 +1443,13 @@
       <c r="F31" s="2">
         <v>1</v>
       </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G31"/>
+      <c r="J31" s="9">
+        <v>551236003045</v>
+      </c>
+      <c r="N31" s="7"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1314,15 +1466,18 @@
         <v>1</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="5">
+      <c r="G32">
+        <v>4620</v>
+      </c>
+      <c r="H32" s="5">
         <v>2360</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>1513215</v>
       </c>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N32" s="7"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1337,9 +1492,10 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G33"/>
+      <c r="N33" s="7"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1356,12 +1512,13 @@
         <v>1</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="H34">
+      <c r="G34"/>
+      <c r="I34">
         <v>1511295</v>
       </c>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N34" s="7"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -1376,12 +1533,18 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="5">
+      <c r="G35">
+        <v>4620</v>
+      </c>
+      <c r="H35" s="5">
         <v>174</v>
       </c>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="9">
+        <v>551236001636</v>
+      </c>
+      <c r="N35" s="7"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1398,11 +1561,15 @@
         <v>1</v>
       </c>
       <c r="F36" s="2"/>
-      <c r="G36" s="5">
+      <c r="G36">
+        <v>4620</v>
+      </c>
+      <c r="H36" s="5">
         <v>1619</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N36" s="7"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -1417,11 +1584,18 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="5">
+      <c r="G37">
+        <v>4620</v>
+      </c>
+      <c r="H37" s="5">
         <v>154</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="9">
+        <v>551236001637</v>
+      </c>
+      <c r="N37" s="7"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1436,11 +1610,18 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="5">
+      <c r="G38">
+        <v>4620</v>
+      </c>
+      <c r="H38" s="5">
         <v>101</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="9">
+        <v>551236003044</v>
+      </c>
+      <c r="N38" s="7"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -1457,11 +1638,13 @@
       <c r="F39" s="2">
         <v>1</v>
       </c>
-      <c r="H39">
+      <c r="G39"/>
+      <c r="I39">
         <v>1507096</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N39" s="7"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -1478,8 +1661,10 @@
         <v>1</v>
       </c>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G40"/>
+      <c r="N40" s="7"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1496,11 +1681,13 @@
         <v>1</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="H41">
+      <c r="G41"/>
+      <c r="I41">
         <v>1507755</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N41" s="7"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -1517,11 +1704,13 @@
         <v>1</v>
       </c>
       <c r="F42" s="2"/>
-      <c r="H42">
+      <c r="G42"/>
+      <c r="I42">
         <v>1506525</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N42" s="7"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -1536,11 +1725,18 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="5">
+      <c r="G43">
+        <v>4620</v>
+      </c>
+      <c r="H43" s="5">
         <v>166</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="9">
+        <v>551236001638</v>
+      </c>
+      <c r="N43" s="7"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1555,11 +1751,15 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="5">
+      <c r="G44">
+        <v>4620</v>
+      </c>
+      <c r="H44" s="5">
         <v>1750</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N44" s="7"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -1574,11 +1774,18 @@
         <v>1</v>
       </c>
       <c r="F45" s="2"/>
-      <c r="G45" s="5">
+      <c r="G45">
+        <v>4620</v>
+      </c>
+      <c r="H45" s="5">
         <v>288</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="9">
+        <v>551236001639</v>
+      </c>
+      <c r="N45" s="7"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1595,11 +1802,18 @@
       <c r="F46" s="2">
         <v>1</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46">
+        <v>4620</v>
+      </c>
+      <c r="H46" s="5">
         <v>800</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="9">
+        <v>551236002471</v>
+      </c>
+      <c r="N46" s="7"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -1616,14 +1830,18 @@
         <v>1</v>
       </c>
       <c r="F47" s="2"/>
-      <c r="G47" s="5">
+      <c r="G47">
+        <v>4620</v>
+      </c>
+      <c r="H47" s="5">
         <v>8540</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>1511433</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N47" s="7"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -1638,11 +1856,18 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="5">
+      <c r="G48">
+        <v>4620</v>
+      </c>
+      <c r="H48" s="5">
         <v>162</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J48" s="9">
+        <v>551236001642</v>
+      </c>
+      <c r="N48" s="7"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -1659,11 +1884,18 @@
       <c r="F49" s="2">
         <v>1</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49">
+        <v>4620</v>
+      </c>
+      <c r="H49" s="5">
         <v>499</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J49" s="9">
+        <v>551236001644</v>
+      </c>
+      <c r="N49" s="7"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -1678,11 +1910,18 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="5">
+      <c r="G50">
+        <v>4620</v>
+      </c>
+      <c r="H50" s="5">
         <v>164</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J50" s="9">
+        <v>551236001646</v>
+      </c>
+      <c r="N50" s="7"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -1699,16 +1938,51 @@
         <v>1</v>
       </c>
       <c r="F51" s="2"/>
-      <c r="G51" s="5">
+      <c r="G51">
+        <v>4620</v>
+      </c>
+      <c r="H51" s="5">
         <v>8722</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>1513496</v>
       </c>
+      <c r="N51" s="7"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="10"/>
+      <c r="G52"/>
+      <c r="N52" s="7"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G53"/>
+      <c r="N53" s="7"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G54"/>
+      <c r="N54" s="7"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G60"/>
     </row>
   </sheetData>
-  <sortState ref="L3:M16">
-    <sortCondition ref="M3:M16"/>
+  <sortState ref="L2:N54">
+    <sortCondition ref="L2:L54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
import and show pss info
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8937309-326F-3D4D-A7C9-DA7D5FB57002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78721161-0774-3D41-9413-7A5F7E515DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2540" windowWidth="27240" windowHeight="16440" xr2:uid="{1F989F6B-AFCF-AF42-9D0E-3D35A3A081C6}"/>
+    <workbookView xWindow="6360" yWindow="2780" windowWidth="27240" windowHeight="16440" xr2:uid="{1F989F6B-AFCF-AF42-9D0E-3D35A3A081C6}"/>
   </bookViews>
   <sheets>
     <sheet name="racine-schools-directory" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="00000"/>
+    <numFmt numFmtId="166" formatCode="00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -314,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -334,6 +335,10 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,14 +655,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C62E933-5DF9-6143-AEAA-89AA45FFA9EF}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.6640625" customWidth="1"/>
     <col min="7" max="8" width="13.83203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="12"/>
     <col min="10" max="10" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.5" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" customWidth="1"/>
@@ -688,7 +694,7 @@
       <c r="H1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="11" t="s">
         <v>65</v>
       </c>
       <c r="J1" s="8" t="s">
@@ -821,7 +827,7 @@
       <c r="H6" s="5">
         <v>1681</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="12" t="s">
         <v>62</v>
       </c>
       <c r="N6" s="7"/>
@@ -980,7 +986,7 @@
       <c r="H12" s="5">
         <v>1711</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="12" t="s">
         <v>63</v>
       </c>
       <c r="N12" s="7"/>
@@ -1106,7 +1112,7 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17"/>
-      <c r="I17">
+      <c r="I17" s="12">
         <v>1507085</v>
       </c>
       <c r="N17" s="7"/>
@@ -1236,7 +1242,7 @@
       <c r="H22" s="5">
         <v>2370</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="12">
         <v>1512696</v>
       </c>
       <c r="N22" s="7"/>
@@ -1339,7 +1345,7 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26"/>
-      <c r="I26" t="s">
+      <c r="I26" s="12" t="s">
         <v>64</v>
       </c>
       <c r="N26" s="7"/>
@@ -1472,7 +1478,7 @@
       <c r="H32" s="5">
         <v>2360</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="12">
         <v>1513215</v>
       </c>
       <c r="N32" s="7"/>
@@ -1513,7 +1519,7 @@
       </c>
       <c r="F34" s="2"/>
       <c r="G34"/>
-      <c r="I34">
+      <c r="I34" s="12">
         <v>1511295</v>
       </c>
       <c r="N34" s="7"/>
@@ -1639,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="G39"/>
-      <c r="I39">
+      <c r="I39" s="12">
         <v>1507096</v>
       </c>
       <c r="N39" s="7"/>
@@ -1682,7 +1688,7 @@
       </c>
       <c r="F41" s="2"/>
       <c r="G41"/>
-      <c r="I41">
+      <c r="I41" s="12">
         <v>1507755</v>
       </c>
       <c r="N41" s="7"/>
@@ -1705,7 +1711,7 @@
       </c>
       <c r="F42" s="2"/>
       <c r="G42"/>
-      <c r="I42">
+      <c r="I42" s="12">
         <v>1506525</v>
       </c>
       <c r="N42" s="7"/>
@@ -1836,7 +1842,7 @@
       <c r="H47" s="5">
         <v>8540</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="12">
         <v>1511433</v>
       </c>
       <c r="N47" s="7"/>
@@ -1944,7 +1950,7 @@
       <c r="H51" s="5">
         <v>8722</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="12">
         <v>1513496</v>
       </c>
       <c r="N51" s="7"/>

</xml_diff>

<commit_message>
add 2 more private schools
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78721161-0774-3D41-9413-7A5F7E515DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699D00F3-08A4-4C46-BC9E-32792CF1EA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="2780" windowWidth="27240" windowHeight="16440" xr2:uid="{1F989F6B-AFCF-AF42-9D0E-3D35A3A081C6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
   <si>
     <t>21st Century Preparatory School</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>District Code</t>
+  </si>
+  <si>
+    <t>Small World Montessori</t>
+  </si>
+  <si>
+    <t>K9306402</t>
+  </si>
+  <si>
+    <t>St John's Lutheran School</t>
   </si>
 </sst>
 </file>
@@ -315,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -339,6 +348,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C62E933-5DF9-6143-AEAA-89AA45FFA9EF}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1956,12 +1968,44 @@
       <c r="N51" s="7"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
+      <c r="A52" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="13">
+        <v>1</v>
+      </c>
       <c r="G52"/>
+      <c r="I52" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="N52" s="7"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="13">
+        <v>8</v>
+      </c>
+      <c r="D53" s="13">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
       <c r="G53"/>
+      <c r="I53" s="12">
+        <v>1511444</v>
+      </c>
       <c r="N53" s="7"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix another data error
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C852435-411F-AC4A-BE42-02EBE19ADFBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0050D6AC-DA74-D04F-BE35-0C31D0FB5424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5440" yWindow="2520" windowWidth="27240" windowHeight="16440" xr2:uid="{1F989F6B-AFCF-AF42-9D0E-3D35A3A081C6}"/>
   </bookViews>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C62E933-5DF9-6143-AEAA-89AA45FFA9EF}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1050,6 +1050,9 @@
       <c r="H14" s="5">
         <v>492</v>
       </c>
+      <c r="J14" s="9">
+        <v>551236001620</v>
+      </c>
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1807,9 +1810,6 @@
         <v>3430</v>
       </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="9">
-        <v>551236001620</v>
-      </c>
       <c r="N44" s="7"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add percent choice to template
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7091C9FF-A181-D848-A643-FBB1B09EE036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F610FE7F-AB89-8043-A510-381D40B628D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24880" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1338,8 +1338,8 @@
   </sheetPr>
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix logos for st schools
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C36D9E16-FA6F-884B-8865-8E98942EF153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19949DF-9808-8B49-A460-20B6522A0D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="31020" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1269,15 +1269,6 @@
     <t>St. Catherines.jpg</t>
   </si>
   <si>
-    <t>St.Joseph.jpg</t>
-  </si>
-  <si>
-    <t>St.Lucy.jpg</t>
-  </si>
-  <si>
-    <t>St.Rita.jpg</t>
-  </si>
-  <si>
     <t>Starbuck (1).jpg</t>
   </si>
   <si>
@@ -1459,6 +1450,15 @@
   </si>
   <si>
     <t>st-johns-logo.jpg</t>
+  </si>
+  <si>
+    <t>St. Rita.jpg</t>
+  </si>
+  <si>
+    <t>St. Lucy.jpg</t>
+  </si>
+  <si>
+    <t>St. Joseph.jpg</t>
   </si>
 </sst>
 </file>
@@ -2530,10 +2530,10 @@
   </sheetPr>
   <dimension ref="A1:BV52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2700,7 +2700,7 @@
         <v>101</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="V2" s="21"/>
       <c r="W2" s="27" t="s">
@@ -2836,7 +2836,7 @@
         <v>88</v>
       </c>
       <c r="U4" s="47" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="V4" s="21"/>
       <c r="W4" s="27" t="s">
@@ -2906,7 +2906,7 @@
         <v>110</v>
       </c>
       <c r="U5" s="21" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="V5" s="21"/>
       <c r="W5" s="27" t="s">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="N7" s="26"/>
       <c r="O7" s="27" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="P7" s="27" t="s">
         <v>342</v>
@@ -3050,7 +3050,7 @@
         <v>128</v>
       </c>
       <c r="U7" s="21" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="V7" s="21"/>
       <c r="W7" s="27" t="s">
@@ -3122,7 +3122,7 @@
         <v>135</v>
       </c>
       <c r="U8" s="21" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="V8" s="21"/>
       <c r="W8" s="27" t="s">
@@ -3192,7 +3192,7 @@
         <v>139</v>
       </c>
       <c r="U9" s="21" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="V9" s="21"/>
       <c r="W9" s="27" t="s">
@@ -3264,7 +3264,7 @@
         <v>143</v>
       </c>
       <c r="U10" s="21" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="V10" s="21"/>
       <c r="W10" s="27" t="s">
@@ -3336,7 +3336,7 @@
         <v>147</v>
       </c>
       <c r="U11" s="21" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="V11" s="21"/>
       <c r="W11" s="27" t="s">
@@ -3408,10 +3408,10 @@
         <v>153</v>
       </c>
       <c r="U12" s="21" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="V12" s="21" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="W12" s="27" t="s">
         <v>154</v>
@@ -3484,7 +3484,7 @@
         <v>158</v>
       </c>
       <c r="U13" s="21" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="V13" s="21"/>
       <c r="W13" s="27" t="s">
@@ -3552,7 +3552,7 @@
         <v>163</v>
       </c>
       <c r="U14" s="21" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="V14" s="21"/>
       <c r="W14" s="27" t="s">
@@ -3622,7 +3622,7 @@
         <v>168</v>
       </c>
       <c r="U15" s="21" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="V15" s="21"/>
       <c r="W15" s="27" t="s">
@@ -3694,7 +3694,7 @@
         <v>173</v>
       </c>
       <c r="U16" s="21" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="V16" s="21"/>
       <c r="W16" s="27" t="s">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="U17" s="21"/>
       <c r="V17" s="21" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="W17" s="27" t="s">
         <v>178</v>
@@ -3838,7 +3838,7 @@
         <v>182</v>
       </c>
       <c r="U18" s="21" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="V18" s="21"/>
       <c r="W18" s="27" t="s">
@@ -3908,7 +3908,7 @@
         <v>186</v>
       </c>
       <c r="U19" s="21" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="V19" s="21"/>
       <c r="W19" s="27" t="s">
@@ -3978,7 +3978,7 @@
         <v>190</v>
       </c>
       <c r="U20" s="21" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="V20" s="21"/>
       <c r="W20" s="27" t="s">
@@ -4048,7 +4048,7 @@
         <v>195</v>
       </c>
       <c r="U21" s="21" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="V21" s="21"/>
       <c r="W21" s="27" t="s">
@@ -4120,7 +4120,7 @@
         <v>199</v>
       </c>
       <c r="U22" s="21" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="V22" s="21"/>
       <c r="W22" s="27" t="s">
@@ -4190,7 +4190,7 @@
         <v>204</v>
       </c>
       <c r="U23" s="21" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="V23" s="21"/>
       <c r="W23" s="27" t="s">
@@ -4260,7 +4260,7 @@
         <v>208</v>
       </c>
       <c r="U24" s="21" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="V24" s="21"/>
       <c r="W24" s="27" t="s">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="W25" s="27" t="s">
         <v>178</v>
@@ -4408,7 +4408,7 @@
         <v>216</v>
       </c>
       <c r="U26" s="30" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="V26" s="30"/>
       <c r="W26" s="36" t="s">
@@ -4603,7 +4603,7 @@
         <v>227</v>
       </c>
       <c r="U28" s="21" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="V28" s="21"/>
       <c r="W28" s="27" t="s">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="W29" s="27" t="s">
         <v>234</v>
@@ -4839,10 +4839,10 @@
         <v>238</v>
       </c>
       <c r="U30" s="21" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="V30" s="21" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="W30" s="27" t="s">
         <v>239</v>
@@ -5079,7 +5079,7 @@
         <v>248</v>
       </c>
       <c r="U32" s="21" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="V32" s="21"/>
       <c r="W32" s="27" t="s">
@@ -5198,10 +5198,10 @@
         <v>254</v>
       </c>
       <c r="U33" s="21" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="V33" s="21" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="W33" s="27" t="s">
         <v>255</v>
@@ -5319,7 +5319,7 @@
         <v>259</v>
       </c>
       <c r="U34" s="21" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="V34" s="21"/>
       <c r="W34" s="27" t="s">
@@ -5436,7 +5436,7 @@
         <v>264</v>
       </c>
       <c r="U35" s="21" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="V35" s="21"/>
       <c r="W35" s="27" t="s">
@@ -5553,10 +5553,10 @@
         <v>268</v>
       </c>
       <c r="U36" s="21" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="V36" s="21" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="W36" s="27" t="s">
         <v>178</v>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="N37" s="26"/>
       <c r="O37" s="27" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="P37" s="27" t="s">
         <v>271</v>
@@ -5769,7 +5769,7 @@
       <c r="M38" s="25"/>
       <c r="N38" s="26"/>
       <c r="O38" s="27" t="s">
-        <v>406</v>
+        <v>469</v>
       </c>
       <c r="P38" s="27" t="s">
         <v>276</v>
@@ -5787,10 +5787,10 @@
         <v>279</v>
       </c>
       <c r="U38" s="21" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="V38" s="21" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="W38" s="27" t="s">
         <v>178</v>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="N39" s="26"/>
       <c r="O39" s="27" t="s">
-        <v>407</v>
+        <v>468</v>
       </c>
       <c r="P39" s="27" t="s">
         <v>283</v>
@@ -5908,10 +5908,10 @@
         <v>286</v>
       </c>
       <c r="U39" s="21" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="V39" s="21" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="W39" s="27" t="s">
         <v>178</v>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="N40" s="26"/>
       <c r="O40" s="27" t="s">
-        <v>408</v>
+        <v>467</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>287</v>
@@ -6029,10 +6029,10 @@
         <v>290</v>
       </c>
       <c r="U40" s="21" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V40" s="21" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="W40" s="27" t="s">
         <v>178</v>
@@ -6150,7 +6150,7 @@
         <v>294</v>
       </c>
       <c r="U41" s="21" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="V41" s="21"/>
       <c r="W41" s="27" t="s">
@@ -6271,10 +6271,10 @@
         <v>297</v>
       </c>
       <c r="U42" s="21" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="V42" s="21" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="W42" s="27" t="s">
         <v>298</v>
@@ -6606,7 +6606,7 @@
         <v>551236002471</v>
       </c>
       <c r="O45" s="27" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="P45" s="27" t="s">
         <v>309</v>
@@ -6624,7 +6624,7 @@
         <v>314</v>
       </c>
       <c r="U45" s="21" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="V45" s="21"/>
       <c r="W45" s="27" t="s">
@@ -6723,7 +6723,7 @@
       <c r="M46" s="25"/>
       <c r="N46" s="26"/>
       <c r="O46" s="27" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="P46" s="27" t="s">
         <v>320</v>
@@ -6741,7 +6741,7 @@
         <v>318</v>
       </c>
       <c r="U46" s="21" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="V46" s="21"/>
       <c r="W46" s="27" t="s">
@@ -6846,7 +6846,7 @@
         <v>551236001642</v>
       </c>
       <c r="O47" s="27" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="P47" s="27" t="s">
         <v>321</v>
@@ -6864,10 +6864,10 @@
         <v>324</v>
       </c>
       <c r="U47" s="21" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="V47" s="21" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="W47" s="27" t="s">
         <v>325</v>
@@ -6985,7 +6985,7 @@
         <v>328</v>
       </c>
       <c r="U48" s="21" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="V48" s="21"/>
       <c r="W48" s="27" t="s">
@@ -7086,7 +7086,7 @@
         <v>551236001646</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="P49" s="27" t="s">
         <v>330</v>
@@ -7104,7 +7104,7 @@
         <v>332</v>
       </c>
       <c r="U49" s="21" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="V49" s="21"/>
       <c r="W49" s="27" t="s">
@@ -7199,7 +7199,7 @@
       <c r="M50" s="25"/>
       <c r="N50" s="26"/>
       <c r="O50" s="27" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="P50" s="27" t="s">
         <v>333</v>
@@ -7217,7 +7217,7 @@
         <v>336</v>
       </c>
       <c r="U50" s="21" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="V50" s="21"/>
       <c r="W50" s="27" t="s">
@@ -7320,7 +7320,7 @@
       </c>
       <c r="N51" s="26"/>
       <c r="O51" s="27" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P51" s="27" t="s">
         <v>337</v>
@@ -7338,10 +7338,10 @@
         <v>340</v>
       </c>
       <c r="U51" s="21" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="V51" s="21" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="W51" s="27" t="s">
         <v>341</v>

</xml_diff>

<commit_message>
update school website url prefixes
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19949DF-9808-8B49-A460-20B6522A0D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CD4AE4-EFDB-6C47-B32A-8719CC13FBFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="31020" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,9 +419,6 @@
     <t>(262) 456-1079</t>
   </si>
   <si>
-    <t>www.evergreen.k12.wi.us</t>
-  </si>
-  <si>
     <t>Each child will be known, valued, challenged, and each day will be in an environment of happiness, joy, and excitement that will generate within them a desire to come to school each day.</t>
   </si>
   <si>
@@ -683,9 +680,6 @@
     <t>(262) 619-4400</t>
   </si>
   <si>
-    <t>www.rusd.org/park</t>
-  </si>
-  <si>
     <t xml:space="preserve">Park is known for its rich tradition of excellence in academics, sports and activities… Its ultimate goal is to have classrooms where students and staff can live and learn in a climate of mutual respect. Further, it will strive to promote an environment where all can take pride in their ethnic and racial heritage. Such goals of respect and understanding have value for development of the greater society in which we all live. </t>
   </si>
   <si>
@@ -704,9 +698,6 @@
     <t>( 262) 752-2500</t>
   </si>
   <si>
-    <t>www.prairieschool.com</t>
-  </si>
-  <si>
     <t>The Prairie School nurtures the creativity, interests and abilities of every student, inspiring each to explore, thrive, and add value individually and in collaboration with others. Our community of students, faculty, and families works together to create a collaborative and supportive culture grounded in human values – celebrating both our differences and commonalities.  Prairie graduates are prepared for college and life with the desire and skills to make the world a better place.</t>
   </si>
   <si>
@@ -716,9 +707,6 @@
     <t>(262) 664-6600</t>
   </si>
   <si>
-    <t>www.rusd.org/alternative-education</t>
-  </si>
-  <si>
     <t>Our mission is to provide alternative pathways for students to meet their graduation requirements through personalized and blended learning. Our vision is that students will acquire the skills to be college and career ready and demonstrate the knowledge, skills and values required to be productive global citizens.</t>
   </si>
   <si>
@@ -731,15 +719,9 @@
     <t>(262) 634-0961</t>
   </si>
   <si>
-    <t>www.racinechristianschool.com</t>
-  </si>
-  <si>
     <t>The Racine Christian School exists to glorify God by providing a Christ-centered education for its students. This education is based upon the infallible Word of God interpreted in conjunction with the confessional statements of the Reformed Churches.</t>
   </si>
   <si>
-    <t>www.ologa.org</t>
-  </si>
-  <si>
     <t>Private, Religious, Christian Schools International</t>
   </si>
   <si>
@@ -749,9 +731,6 @@
     <t>(262) 637-6538</t>
   </si>
   <si>
-    <t>www.racinelutheran.org</t>
-  </si>
-  <si>
     <t>Racine Lutheran High School’s mission is to guide our youth in faith, learning, character and leadership by nurturing their relationship with Jesus Christ, and educating them for a life of service to God and man.</t>
   </si>
   <si>
@@ -764,9 +743,6 @@
     <t>(262) 637-7802</t>
   </si>
   <si>
-    <t>www.racinemontessori.com</t>
-  </si>
-  <si>
     <t>Montessori is a hands-on approach to learning. It encourages children to develop their observation skills through activities that use the five senses, kinetic movement, spatial refinement, small and gross motor skill coordination, and concrete knowledge that leads to later abstraction.</t>
   </si>
   <si>
@@ -777,9 +753,6 @@
   </si>
   <si>
     <t>(262) 619-4500</t>
-  </si>
-  <si>
-    <t>www.risd.org/redapple-es</t>
   </si>
   <si>
     <t>Through STEAM, Red Apple Elementary engages, inspires and empowers a community of learners in critical thinking, collaboration and innovation; preparing students to be college and/or career ready in alignment with the [RUSD] North Star vision.</t>
@@ -804,9 +777,6 @@
 (262) 634-3010</t>
   </si>
   <si>
-    <t>www.luminschools.org/LUMIN-Schools/Our-Schools/Renaissance-School.htm</t>
-  </si>
-  <si>
     <t>Our purpose is to provide safe, Christian schools focused on educational success, leadership development and spiritual growth. We help our students work hard to achieve greatness by nurturing and equipping them in a strong Christian and academic environment to become lifelong learners, capable of making responsible decisions, growing in faith and serving God and the community.</t>
   </si>
   <si>
@@ -819,9 +789,6 @@
     <t>(262) 664-8300</t>
   </si>
   <si>
-    <t>www.rusd.org/roosevelt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Roosevelt Elementary School is a positive learning community where every student and staff member strives to become collaboratively focused on maximum student academic, social and emotional growth in order to meet the RUSD North Star goals. Roosevelt is a neighborhood school with a lot of heart. </t>
   </si>
   <si>
@@ -834,9 +801,6 @@
     <t>(262) 664-6850</t>
   </si>
   <si>
-    <t>www.rusd.org/montessori</t>
-  </si>
-  <si>
     <t xml:space="preserve">Montessori education is a method of education based on self-directed learning activities that emphasize learning through all five senses and multi-age classrooms. Children in Montessori classes learn at their own, individual pace and according to their own choice of activities from hundreds of possibilities. Learning is an exciting process of discovery, leading to concentration, coordination, motivation, self-discipline, and independence.  </t>
   </si>
   <si>
@@ -846,9 +810,6 @@
     <t>(262) 632-2785</t>
   </si>
   <si>
-    <t>www.saintcats.org</t>
-  </si>
-  <si>
     <t>St. Catherine’s educates students in the Catholic faith, fostering an environment of academic and behavioral excellence to create lifelong learners and globally responsible citizens. St. Catherine’s is built on the Dominican values of Study, Prayer, Service and Community.</t>
   </si>
   <si>
@@ -864,9 +825,6 @@
     <t>(262) 633-2758</t>
   </si>
   <si>
-    <t>www.stjohnsracine.org</t>
-  </si>
-  <si>
     <t>At St. John's Lutheran School, we provide an educational environment that strives to enrich the "whole" child in a "holy" way. We challenge the academic development of all children in a setting that nurtures the gifts each child has been given by God. Our spiritual climate encourages an active faith in Jesus Christ, our Lord and Savior. Our students in 3-year old preschool to 8th grade are daily challenged by caring teachers to stretch both their minds and hearts in a grace filled environment.</t>
   </si>
   <si>
@@ -879,9 +837,6 @@
     <t>(262) 633-2403</t>
   </si>
   <si>
-    <t>www.st-joes-school.org</t>
-  </si>
-  <si>
     <t>Catholic schools in the Archdiocese of Milwaukee uniquely balance faith and education. We do more than prepare students for tests in the classroom. We prepare them for tests in life. Students participate in daily prayer and religion classes, have frequent opportunities for worship and Mass attendance, and receive sacramental preparation. Students are taught to be respectful and compassionate, and emphasis is placed not only on academic achievement, but on moral and spiritual growth.</t>
   </si>
   <si>
@@ -900,9 +855,6 @@
     <t>(262) 554-1801 X211</t>
   </si>
   <si>
-    <t>www.stlucysschool.com</t>
-  </si>
-  <si>
     <t>St. Lucy Catholic Parish School is a community of parents, students, parishioners, and staff faithful to the teachings of the Catholic Church, providing a full range of educational programs inspired by the Gospel message.</t>
   </si>
   <si>
@@ -912,9 +864,6 @@
     <t>(262) 639-3333</t>
   </si>
   <si>
-    <t>www.st-ritasschool.org</t>
-  </si>
-  <si>
     <t>Our identity as a Catholic school is woven into every aspect of school life. Each child's personal relationship with Jesus is forefront. We foster this relationship with daily religion class, daily prayer, weekly mass, and seasonal religious activities. We encourage our families to carry on this mission at home by attending mass each weekend and setting and achieving faith goals.</t>
   </si>
   <si>
@@ -924,18 +873,12 @@
     <t>(262) 664-6300</t>
   </si>
   <si>
-    <t>www.rusd.org/schulte</t>
-  </si>
-  <si>
     <t>"It's all about the kids."  At Schulte, it is our staff's responsibility to provide a child-centered school community that is both academically challenging and supportive. All students will reach their individual potential and make a positive impact on society.</t>
   </si>
   <si>
     <t>245 Main Street, Suite L-2</t>
   </si>
   <si>
-    <t>www.sienacatholicschools.org</t>
-  </si>
-  <si>
     <t>Siena Catholic Schools of Racine unites the area’s five Catholic elementary schools (John Paul II Academy, Our Lady of Grace Academy, St. Joseph, St. Lucy, St. Rita) and one middle/high school (St. Catherine’s) in a regional model of Catholic education intended to preserve the individual identity, history and uniqueness of each school while maximizing the impact of collective strength. We are committed to educating in a Catholic learning environment rooted in Christ’s teachings and characterized by academic excellence, servant leadership, student diversity, personal accountability and respect for every individual.</t>
   </si>
   <si>
@@ -948,9 +891,6 @@
     <t>(262) 632-6797</t>
   </si>
   <si>
-    <t>www.swmschool.org</t>
-  </si>
-  <si>
     <t>Provide a safe, home-like atmosphere for your children to learn.</t>
   </si>
   <si>
@@ -966,9 +906,6 @@
     <t>(262) 671-5015</t>
   </si>
   <si>
-    <t>www.sonnenbergschool.com</t>
-  </si>
-  <si>
     <t>Our mission at Sonnenberg School is to provide an educational environment that is loving, safe, and supportive, focused on preparing students academically, socially, and emotionally for their future lives of success. Designed specifically to meet the needs of students on the Autism Spectrum, Sonnenberg School ensures that all students receive an outstanding education from highly qualified and caring teachers. We work to help every child develop his or her unique gifts and talents to the fullest potential.</t>
   </si>
   <si>
@@ -981,12 +918,6 @@
     <t>www.rusd.org/starbuck</t>
   </si>
   <si>
-    <t>www.rusd.org/wadewitz</t>
-  </si>
-  <si>
-    <t>www.rusd.org/walden</t>
-  </si>
-  <si>
     <t>Starbuck Middle School is an International Baccalaureate (IB) World School for the Middle Years Programme (MYP). The IB MYP is a framework for teaching that benefits all students. It addresses a wide variety of learning styles, involves all students in their own unique learning processes and gives students a standard, internationally accepted foundation of knowledge.… Students who participate in the IB MYP become independent learners who can recognize relationships between school subjects and the world outside. Through the IB Programme, Starbuck offers an inquiry-based curriculum that empowers students to become responsible world citizens and lifelong learners.</t>
   </si>
   <si>
@@ -996,9 +927,6 @@
     <t>(262) 664-6100</t>
   </si>
   <si>
-    <t>www.rusd.org/real</t>
-  </si>
-  <si>
     <t>The mission of the Racine Engineering Arts and Leadership (REAL) School is to motivate every student to assume accountability for his/her own educational process while becoming a joyful lifelong learner and successful in careers and family. Every student will have a purpose and identity that drives their self-confidence and skill development necessary to succeed in life.</t>
   </si>
   <si>
@@ -1014,9 +942,6 @@
     <t>(262) 632-2900</t>
   </si>
   <si>
-    <t>www.trinityracine.com/primary-school</t>
-  </si>
-  <si>
     <t xml:space="preserve">The mission of Trinity Lutheran School is to partner with parents to guide and educate children and families to know that they are redeemed children of God. As such, through education, they will identify, develop, and utilize their God-given talents, thereby preparing them to spread the good news of Jesus Christ to all nations and serve their neighbor. </t>
   </si>
   <si>
@@ -1050,9 +975,6 @@
     <t>(262) 664-6200</t>
   </si>
   <si>
-    <t>www.rusd.org/westridge</t>
-  </si>
-  <si>
     <t>The mission of West Ridge is to provide a rigorous, relevant and inquiry-based educational environment that challenges students to excel. We embrace a partnership with students, parents, educators and members of our community to attain these goals. West Ridge is an elementary IB (International Baccalaureate) school. International Baccalaureate (IB) is a nonprofit, educational foundation that offers three different educational programs that help students develop the intellectual, academic, personal, emotional and social skills to live, learn and work in a rapidly globalizing world.</t>
   </si>
   <si>
@@ -1060,9 +982,6 @@
   </si>
   <si>
     <t>(262) 456-2770</t>
-  </si>
-  <si>
-    <t>www.wisconsinlutheranschool.org</t>
   </si>
   <si>
     <t>We seek to prepare children for eternity by learning about Jesus and his forgiveness. We also seek to develop good citizens for our community and country. Jesus stated that these are the greatest of all the commandments: "Love the Lord your God with all your heart and with all your soul and with all your strength and with all your mind" and "Love your neighbor as yourself." We seek to instill this in our children by example and instruction. The Lord is gracious to promise that he will see that all other things are added to us according to our needs. (Matthew 6:33)</t>
@@ -1459,6 +1378,87 @@
   </si>
   <si>
     <t>St. Joseph.jpg</t>
+  </si>
+  <si>
+    <t>http://www.evergreen.k12.wi.us</t>
+  </si>
+  <si>
+    <t>http://www.ologa.org</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/park</t>
+  </si>
+  <si>
+    <t>https://www.prairieschool.com</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/alternative-education</t>
+  </si>
+  <si>
+    <t>https://www.racinechristianschool.com</t>
+  </si>
+  <si>
+    <t>http://www.racinelutheran.org</t>
+  </si>
+  <si>
+    <t>https://www.racinemontessori.com</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/redapple-es</t>
+  </si>
+  <si>
+    <t>https://www.luminschools.org/LUMIN-Schools/Our-Schools/Renaissance-School.htm</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/roosevelt</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/montessori</t>
+  </si>
+  <si>
+    <t>https://www.saintcats.org</t>
+  </si>
+  <si>
+    <t>https://www.stjohnsracine.org</t>
+  </si>
+  <si>
+    <t>http://www.st-joes-school.org</t>
+  </si>
+  <si>
+    <t>https://www.stlucysschool.com</t>
+  </si>
+  <si>
+    <t>https://www.st-ritasschool.org</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/schulte</t>
+  </si>
+  <si>
+    <t>https://www.sienacatholicschools.org</t>
+  </si>
+  <si>
+    <t>https://www.swmschool.org</t>
+  </si>
+  <si>
+    <t>https://www.sonnenbergschool.com</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/real</t>
+  </si>
+  <si>
+    <t>http://www.trinityracine.com/primary-school</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/wadewitz</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/walden</t>
+  </si>
+  <si>
+    <t>https://www.rusd.org/westridge</t>
+  </si>
+  <si>
+    <t>https://www.wisconsinlutheranschool.org</t>
   </si>
 </sst>
 </file>
@@ -2530,10 +2530,10 @@
   </sheetPr>
   <dimension ref="A1:BV52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="O40" sqref="O1:O1048576"/>
+      <selection pane="bottomLeft" activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2682,7 +2682,7 @@
         <v>550004502575</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>97</v>
@@ -2700,7 +2700,7 @@
         <v>101</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>413</v>
+        <v>386</v>
       </c>
       <c r="V2" s="21"/>
       <c r="W2" s="27" t="s">
@@ -2750,7 +2750,7 @@
       <c r="M3" s="22"/>
       <c r="N3" s="26"/>
       <c r="O3" s="27" t="s">
-        <v>368</v>
+        <v>341</v>
       </c>
       <c r="P3" s="27" t="s">
         <v>102</v>
@@ -2818,7 +2818,7 @@
         <v>551236001621</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="P4" s="28" t="s">
         <v>84</v>
@@ -2836,7 +2836,7 @@
         <v>88</v>
       </c>
       <c r="U4" s="47" t="s">
-        <v>415</v>
+        <v>388</v>
       </c>
       <c r="V4" s="21"/>
       <c r="W4" s="27" t="s">
@@ -2888,7 +2888,7 @@
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
       <c r="O5" s="27" t="s">
-        <v>369</v>
+        <v>342</v>
       </c>
       <c r="P5" s="27" t="s">
         <v>107</v>
@@ -2906,7 +2906,7 @@
         <v>110</v>
       </c>
       <c r="U5" s="21" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
       <c r="V5" s="21"/>
       <c r="W5" s="27" t="s">
@@ -2960,7 +2960,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="26"/>
       <c r="O6" s="27" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
       <c r="P6" s="27" t="s">
         <v>119</v>
@@ -3032,29 +3032,29 @@
       </c>
       <c r="N7" s="26"/>
       <c r="O7" s="27" t="s">
-        <v>412</v>
+        <v>385</v>
       </c>
       <c r="P7" s="27" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="Q7" s="27" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="R7" s="27" t="s">
         <v>126</v>
       </c>
       <c r="S7" s="39" t="s">
+        <v>443</v>
+      </c>
+      <c r="T7" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="T7" s="27" t="s">
-        <v>128</v>
-      </c>
       <c r="U7" s="21" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="V7" s="21"/>
       <c r="W7" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X7" s="27">
         <v>351</v>
@@ -3063,7 +3063,7 @@
         <v>76.599999999999994</v>
       </c>
       <c r="Z7" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA7" s="27">
         <v>98</v>
@@ -3104,25 +3104,25 @@
         <v>551236001611</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="P8" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="Q8" s="27" t="s">
+      <c r="R8" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="S8" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="S8" s="39" t="s">
+      <c r="T8" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="T8" s="27" t="s">
-        <v>135</v>
-      </c>
       <c r="U8" s="21" t="s">
-        <v>417</v>
+        <v>390</v>
       </c>
       <c r="V8" s="21"/>
       <c r="W8" s="27" t="s">
@@ -3135,7 +3135,7 @@
         <v>81.7</v>
       </c>
       <c r="Z8" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA8" s="27"/>
     </row>
@@ -3145,7 +3145,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>1</v>
@@ -3174,25 +3174,25 @@
         <v>551236001614</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="P9" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q9" s="27" t="s">
         <v>85</v>
       </c>
       <c r="R9" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="S9" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="S9" s="39" t="s">
+      <c r="T9" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="T9" s="27" t="s">
-        <v>139</v>
-      </c>
       <c r="U9" s="21" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
       <c r="V9" s="21"/>
       <c r="W9" s="27" t="s">
@@ -3205,7 +3205,7 @@
         <v>83.6</v>
       </c>
       <c r="Z9" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA9" s="27"/>
     </row>
@@ -3215,7 +3215,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>1</v>
@@ -3246,25 +3246,25 @@
         <v>551236002311</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="P10" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q10" s="27" t="s">
         <v>85</v>
       </c>
       <c r="R10" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="S10" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="S10" s="39" t="s">
+      <c r="T10" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="T10" s="27" t="s">
-        <v>143</v>
-      </c>
       <c r="U10" s="21" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="V10" s="21"/>
       <c r="W10" s="27" t="s">
@@ -3277,7 +3277,7 @@
         <v>28.9</v>
       </c>
       <c r="Z10" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA10" s="27"/>
     </row>
@@ -3287,7 +3287,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>25</v>
@@ -3318,25 +3318,25 @@
         <v>551236001608</v>
       </c>
       <c r="O11" s="27" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="P11" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q11" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R11" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="S11" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="S11" s="39" t="s">
+      <c r="T11" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="T11" s="27" t="s">
-        <v>147</v>
-      </c>
       <c r="U11" s="21" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="V11" s="21"/>
       <c r="W11" s="27" t="s">
@@ -3349,7 +3349,7 @@
         <v>57</v>
       </c>
       <c r="Z11" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AA11" s="27"/>
     </row>
@@ -3390,31 +3390,31 @@
       <c r="M12" s="25"/>
       <c r="N12" s="26"/>
       <c r="O12" s="27" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
       <c r="P12" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q12" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="Q12" s="27" t="s">
+      <c r="R12" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="R12" s="27" t="s">
+      <c r="S12" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="S12" s="39" t="s">
+      <c r="T12" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="T12" s="27" t="s">
+      <c r="U12" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="V12" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="W12" s="27" t="s">
         <v>153</v>
-      </c>
-      <c r="U12" s="21" t="s">
-        <v>422</v>
-      </c>
-      <c r="V12" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="W12" s="27" t="s">
-        <v>154</v>
       </c>
       <c r="X12" s="27">
         <v>319</v>
@@ -3423,7 +3423,7 @@
         <v>84.6</v>
       </c>
       <c r="Z12" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA12" s="27">
         <v>99.7</v>
@@ -3466,25 +3466,25 @@
         <v>551236001620</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>376</v>
+        <v>349</v>
       </c>
       <c r="P13" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q13" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R13" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="S13" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="S13" s="39" t="s">
+      <c r="T13" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="T13" s="27" t="s">
-        <v>158</v>
-      </c>
       <c r="U13" s="21" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="V13" s="21"/>
       <c r="W13" s="27" t="s">
@@ -3497,7 +3497,7 @@
         <v>63.5</v>
       </c>
       <c r="Z13" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA13" s="27"/>
     </row>
@@ -3534,25 +3534,25 @@
       <c r="M14" s="25"/>
       <c r="N14" s="26"/>
       <c r="O14" s="27" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="P14" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q14" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="R14" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="Q14" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="R14" s="27" t="s">
+      <c r="S14" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="S14" s="39" t="s">
+      <c r="T14" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="T14" s="27" t="s">
-        <v>163</v>
-      </c>
       <c r="U14" s="21" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="V14" s="21"/>
       <c r="W14" s="27" t="s">
@@ -3565,7 +3565,7 @@
         <v>93.9</v>
       </c>
       <c r="Z14" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA14" s="27"/>
     </row>
@@ -3575,7 +3575,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>25</v>
@@ -3604,25 +3604,25 @@
         <v>551236001622</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="P15" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q15" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R15" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="S15" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="S15" s="39" t="s">
+      <c r="T15" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="T15" s="27" t="s">
-        <v>168</v>
-      </c>
       <c r="U15" s="21" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="V15" s="21"/>
       <c r="W15" s="27" t="s">
@@ -3635,7 +3635,7 @@
         <v>41.2</v>
       </c>
       <c r="Z15" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AA15" s="27"/>
     </row>
@@ -3645,7 +3645,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>363</v>
+        <v>336</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>1</v>
@@ -3676,25 +3676,25 @@
         <v>551236001623</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>379</v>
+        <v>352</v>
       </c>
       <c r="P16" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q16" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="R16" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="S16" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="Q16" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="R16" s="27" t="s">
+      <c r="T16" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="S16" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="T16" s="27" t="s">
-        <v>173</v>
-      </c>
       <c r="U16" s="21" t="s">
-        <v>427</v>
+        <v>400</v>
       </c>
       <c r="V16" s="21"/>
       <c r="W16" s="27" t="s">
@@ -3707,7 +3707,7 @@
         <v>77.3</v>
       </c>
       <c r="Z16" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA16" s="27"/>
     </row>
@@ -3752,35 +3752,35 @@
         <v>551236001624</v>
       </c>
       <c r="O17" s="27" t="s">
-        <v>389</v>
+        <v>362</v>
       </c>
       <c r="P17" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q17" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R17" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="S17" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="S17" s="39" t="s">
+      <c r="T17" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="T17" s="27" t="s">
-        <v>177</v>
       </c>
       <c r="U17" s="21"/>
       <c r="V17" s="21" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="W17" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X17" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Y17" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z17" s="27" t="s">
         <v>125</v>
@@ -3795,7 +3795,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>1</v>
@@ -3820,25 +3820,25 @@
       </c>
       <c r="N18" s="26"/>
       <c r="O18" s="27" t="s">
-        <v>390</v>
+        <v>363</v>
       </c>
       <c r="P18" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q18" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="R18" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="Q18" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="R18" s="27" t="s">
+      <c r="S18" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="S18" s="39" t="s">
+      <c r="T18" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="T18" s="27" t="s">
-        <v>182</v>
-      </c>
       <c r="U18" s="21" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
       <c r="V18" s="21"/>
       <c r="W18" s="27" t="s">
@@ -3851,7 +3851,7 @@
         <v>85.2</v>
       </c>
       <c r="Z18" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA18" s="27"/>
     </row>
@@ -3861,7 +3861,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>1</v>
@@ -3890,25 +3890,25 @@
         <v>551236001626</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="P19" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q19" s="27" t="s">
         <v>103</v>
       </c>
       <c r="R19" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="S19" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="S19" s="39" t="s">
+      <c r="T19" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="T19" s="27" t="s">
-        <v>186</v>
-      </c>
       <c r="U19" s="21" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="V19" s="21"/>
       <c r="W19" s="27" t="s">
@@ -3921,7 +3921,7 @@
         <v>81.099999999999994</v>
       </c>
       <c r="Z19" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA19" s="27"/>
     </row>
@@ -3931,7 +3931,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>1</v>
@@ -3960,25 +3960,25 @@
         <v>551236001627</v>
       </c>
       <c r="O20" s="27" t="s">
-        <v>391</v>
+        <v>364</v>
       </c>
       <c r="P20" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q20" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R20" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="S20" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="S20" s="39" t="s">
+      <c r="T20" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="T20" s="27" t="s">
-        <v>190</v>
-      </c>
       <c r="U20" s="21" t="s">
-        <v>431</v>
+        <v>404</v>
       </c>
       <c r="V20" s="21"/>
       <c r="W20" s="27" t="s">
@@ -3991,7 +3991,7 @@
         <v>94.3</v>
       </c>
       <c r="Z20" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AA20" s="27"/>
     </row>
@@ -4001,7 +4001,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>1</v>
@@ -4030,25 +4030,25 @@
         <v>551236003337</v>
       </c>
       <c r="O21" s="27" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="P21" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q21" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="R21" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="Q21" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="R21" s="27" t="s">
+      <c r="S21" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="S21" s="39" t="s">
+      <c r="T21" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="T21" s="27" t="s">
-        <v>195</v>
-      </c>
       <c r="U21" s="21" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
       <c r="V21" s="21"/>
       <c r="W21" s="27" t="s">
@@ -4061,7 +4061,7 @@
         <v>87.8</v>
       </c>
       <c r="Z21" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AA21" s="27"/>
     </row>
@@ -4102,25 +4102,25 @@
         <v>551236001628</v>
       </c>
       <c r="O22" s="27" t="s">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="P22" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q22" s="27" t="s">
         <v>103</v>
       </c>
       <c r="R22" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="S22" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="S22" s="39" t="s">
+      <c r="T22" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="T22" s="27" t="s">
-        <v>199</v>
-      </c>
       <c r="U22" s="21" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
       <c r="V22" s="21"/>
       <c r="W22" s="27" t="s">
@@ -4133,7 +4133,7 @@
         <v>80.8</v>
       </c>
       <c r="Z22" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AA22" s="27"/>
     </row>
@@ -4172,25 +4172,25 @@
       </c>
       <c r="N23" s="26"/>
       <c r="O23" s="27" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="P23" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q23" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="R23" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="Q23" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="R23" s="27" t="s">
+      <c r="S23" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="S23" s="39" t="s">
+      <c r="T23" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="T23" s="27" t="s">
-        <v>204</v>
-      </c>
       <c r="U23" s="21" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
       <c r="V23" s="21"/>
       <c r="W23" s="27" t="s">
@@ -4203,7 +4203,7 @@
         <v>77.7</v>
       </c>
       <c r="Z23" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA23" s="27"/>
     </row>
@@ -4242,25 +4242,25 @@
         <v>551236001632</v>
       </c>
       <c r="O24" s="27" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="P24" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q24" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="R24" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="Q24" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="R24" s="27" t="s">
+      <c r="S24" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="S24" s="39" t="s">
+      <c r="T24" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="T24" s="27" t="s">
-        <v>208</v>
-      </c>
       <c r="U24" s="21" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="V24" s="21"/>
       <c r="W24" s="27" t="s">
@@ -4273,7 +4273,7 @@
         <v>42.2</v>
       </c>
       <c r="Z24" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA24" s="27"/>
     </row>
@@ -4318,35 +4318,35 @@
         <v>551236001634</v>
       </c>
       <c r="O25" s="27" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="P25" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q25" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="R25" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="Q25" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="R25" s="27" t="s">
+      <c r="S25" s="43" t="s">
+        <v>444</v>
+      </c>
+      <c r="T25" s="27" t="s">
         <v>210</v>
-      </c>
-      <c r="S25" s="43" t="s">
-        <v>233</v>
-      </c>
-      <c r="T25" s="27" t="s">
-        <v>211</v>
       </c>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="W25" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X25" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y25" s="42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Z25" s="27" t="s">
         <v>125</v>
@@ -4390,25 +4390,25 @@
         <v>551236001605</v>
       </c>
       <c r="O26" s="36" t="s">
-        <v>382</v>
+        <v>355</v>
       </c>
       <c r="P26" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q26" s="36" t="s">
         <v>103</v>
       </c>
       <c r="R26" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="S26" s="39" t="s">
+        <v>445</v>
+      </c>
+      <c r="T26" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="S26" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="T26" s="36" t="s">
-        <v>216</v>
-      </c>
       <c r="U26" s="30" t="s">
-        <v>439</v>
+        <v>412</v>
       </c>
       <c r="V26" s="30"/>
       <c r="W26" s="36" t="s">
@@ -4421,7 +4421,7 @@
         <v>71.900000000000006</v>
       </c>
       <c r="Z26" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA26" s="36"/>
     </row>
@@ -4431,7 +4431,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="C27" s="22">
         <v>5</v>
@@ -4453,7 +4453,7 @@
       <c r="J27" s="22"/>
       <c r="K27" s="23"/>
       <c r="L27" s="24" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="M27" s="25" t="s">
         <v>75</v>
@@ -4462,22 +4462,22 @@
         <v>551236001635</v>
       </c>
       <c r="O27" s="27" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="P27" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q27" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="R27" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="S27" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="T27" s="27" t="s">
         <v>220</v>
-      </c>
-      <c r="Q27" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="R27" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="S27" s="39" t="s">
-        <v>222</v>
-      </c>
-      <c r="T27" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="U27" s="21" t="s">
         <v>115</v>
@@ -4493,7 +4493,7 @@
         <v>114</v>
       </c>
       <c r="Z27" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA27" s="27" t="s">
         <v>114</v>
@@ -4585,25 +4585,25 @@
         <v>551236003045</v>
       </c>
       <c r="O28" s="27" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
       <c r="P28" s="27" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q28" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R28" s="27" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="S28" s="44" t="s">
-        <v>226</v>
+        <v>447</v>
       </c>
       <c r="T28" s="27" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="U28" s="21" t="s">
-        <v>441</v>
+        <v>414</v>
       </c>
       <c r="V28" s="21"/>
       <c r="W28" s="27" t="s">
@@ -4616,7 +4616,7 @@
         <v>81.7</v>
       </c>
       <c r="Z28" s="27" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AA28" s="27"/>
       <c r="AB28"/>
@@ -4706,29 +4706,29 @@
       </c>
       <c r="N29" s="26"/>
       <c r="O29" s="27" t="s">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="P29" s="27" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="Q29" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R29" s="27" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="S29" s="45" t="s">
-        <v>231</v>
+        <v>448</v>
       </c>
       <c r="T29" s="27" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21" t="s">
-        <v>442</v>
+        <v>415</v>
       </c>
       <c r="W29" s="27" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="X29" s="27">
         <v>61</v>
@@ -4821,31 +4821,31 @@
       <c r="M30" s="25"/>
       <c r="N30" s="26"/>
       <c r="O30" s="27" t="s">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="P30" s="27" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="Q30" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R30" s="27" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="S30" s="39" t="s">
-        <v>237</v>
+        <v>449</v>
       </c>
       <c r="T30" s="27" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="U30" s="21" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
       <c r="V30" s="21" t="s">
-        <v>434</v>
+        <v>407</v>
       </c>
       <c r="W30" s="27" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="X30" s="27">
         <v>264</v>
@@ -4942,22 +4942,22 @@
       </c>
       <c r="N31" s="26"/>
       <c r="O31" s="27" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="P31" s="27" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q31" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="S31" s="39" t="s">
-        <v>242</v>
+        <v>450</v>
       </c>
       <c r="T31" s="27" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="U31" s="21" t="s">
         <v>114</v>
@@ -4973,7 +4973,7 @@
         <v>114</v>
       </c>
       <c r="Z31" s="27" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="AA31" s="27" t="s">
         <v>114</v>
@@ -5032,7 +5032,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>1</v>
@@ -5061,25 +5061,25 @@
         <v>551236001636</v>
       </c>
       <c r="O32" s="27" t="s">
-        <v>402</v>
+        <v>375</v>
       </c>
       <c r="P32" s="27" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="Q32" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="S32" s="39" t="s">
-        <v>247</v>
+        <v>451</v>
       </c>
       <c r="T32" s="27" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="U32" s="21" t="s">
-        <v>443</v>
+        <v>416</v>
       </c>
       <c r="V32" s="21"/>
       <c r="W32" s="27" t="s">
@@ -5092,7 +5092,7 @@
         <v>52.1</v>
       </c>
       <c r="Z32" s="27" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="AA32" s="27"/>
       <c r="AB32"/>
@@ -5180,31 +5180,31 @@
       <c r="M33" s="25"/>
       <c r="N33" s="26"/>
       <c r="O33" s="27" t="s">
-        <v>383</v>
+        <v>356</v>
       </c>
       <c r="P33" s="27" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="Q33" s="27" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="R33" s="27" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="S33" s="48" t="s">
-        <v>253</v>
+        <v>452</v>
       </c>
       <c r="T33" s="27" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="U33" s="21" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
       <c r="V33" s="21" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
       <c r="W33" s="27" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="X33" s="27">
         <v>346</v>
@@ -5272,7 +5272,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>1</v>
@@ -5301,25 +5301,25 @@
         <v>551236001637</v>
       </c>
       <c r="O34" s="27" t="s">
-        <v>384</v>
+        <v>357</v>
       </c>
       <c r="P34" s="27" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="Q34" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R34" s="27" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="S34" s="39" t="s">
-        <v>258</v>
+        <v>453</v>
       </c>
       <c r="T34" s="27" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="U34" s="21" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="V34" s="21"/>
       <c r="W34" s="27" t="s">
@@ -5332,7 +5332,7 @@
         <v>87.4</v>
       </c>
       <c r="Z34" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA34" s="27"/>
       <c r="AB34"/>
@@ -5389,7 +5389,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>1</v>
@@ -5418,25 +5418,25 @@
         <v>551236003044</v>
       </c>
       <c r="O35" s="27" t="s">
-        <v>403</v>
+        <v>376</v>
       </c>
       <c r="P35" s="27" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="Q35" s="27" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="R35" s="27" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="S35" s="39" t="s">
-        <v>263</v>
+        <v>454</v>
       </c>
       <c r="T35" s="27" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="U35" s="21" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="V35" s="21"/>
       <c r="W35" s="27" t="s">
@@ -5449,7 +5449,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="Z35" s="27" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="AA35" s="27"/>
       <c r="AB35"/>
@@ -5535,34 +5535,34 @@
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="27" t="s">
-        <v>405</v>
+        <v>378</v>
       </c>
       <c r="P36" s="27" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="Q36" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R36" s="27" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="S36" s="39" t="s">
-        <v>267</v>
+        <v>455</v>
       </c>
       <c r="T36" s="27" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="U36" s="21" t="s">
-        <v>460</v>
+        <v>433</v>
       </c>
       <c r="V36" s="21" t="s">
-        <v>461</v>
+        <v>434</v>
       </c>
       <c r="W36" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X36" s="27" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="Y36" s="21">
         <v>51.9</v>
@@ -5571,7 +5571,7 @@
         <v>125</v>
       </c>
       <c r="AA36" s="27" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="AB36"/>
       <c r="AC36"/>
@@ -5652,27 +5652,27 @@
       </c>
       <c r="N37" s="26"/>
       <c r="O37" s="27" t="s">
-        <v>466</v>
+        <v>439</v>
       </c>
       <c r="P37" s="27" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="Q37" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R37" s="27" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="S37" s="39" t="s">
-        <v>273</v>
+        <v>456</v>
       </c>
       <c r="T37" s="27" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21"/>
       <c r="W37" s="27" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="X37" s="27">
         <v>222</v>
@@ -5769,43 +5769,43 @@
       <c r="M38" s="25"/>
       <c r="N38" s="26"/>
       <c r="O38" s="27" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="P38" s="27" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="Q38" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R38" s="27" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="S38" s="39" t="s">
-        <v>278</v>
+        <v>457</v>
       </c>
       <c r="T38" s="27" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="U38" s="21" t="s">
-        <v>447</v>
+        <v>420</v>
       </c>
       <c r="V38" s="21" t="s">
-        <v>448</v>
+        <v>421</v>
       </c>
       <c r="W38" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X38" s="27" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="Y38" s="21" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="Z38" s="27" t="s">
         <v>125</v>
       </c>
       <c r="AA38" s="27" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="AB38"/>
       <c r="AC38"/>
@@ -5861,7 +5861,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>404</v>
+        <v>377</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>28</v>
@@ -5890,31 +5890,31 @@
       </c>
       <c r="N39" s="26"/>
       <c r="O39" s="27" t="s">
-        <v>468</v>
+        <v>441</v>
       </c>
       <c r="P39" s="27" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="Q39" s="27" t="s">
         <v>103</v>
       </c>
       <c r="R39" s="27" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="S39" s="39" t="s">
-        <v>285</v>
+        <v>458</v>
       </c>
       <c r="T39" s="27" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="U39" s="21" t="s">
-        <v>462</v>
+        <v>435</v>
       </c>
       <c r="V39" s="21" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="W39" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X39" s="27">
         <v>190</v>
@@ -5982,7 +5982,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>25</v>
@@ -6011,31 +6011,31 @@
       </c>
       <c r="N40" s="26"/>
       <c r="O40" s="27" t="s">
-        <v>467</v>
+        <v>440</v>
       </c>
       <c r="P40" s="27" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="Q40" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R40" s="27" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="S40" s="39" t="s">
-        <v>289</v>
+        <v>459</v>
       </c>
       <c r="T40" s="27" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="U40" s="21" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="V40" s="21" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="W40" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X40" s="27">
         <v>148</v>
@@ -6103,7 +6103,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>360</v>
+        <v>333</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>1</v>
@@ -6132,25 +6132,25 @@
         <v>551236001638</v>
       </c>
       <c r="O41" s="27" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
       <c r="P41" s="27" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="Q41" s="27" t="s">
         <v>120</v>
       </c>
       <c r="R41" s="27" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="S41" s="39" t="s">
-        <v>293</v>
+        <v>460</v>
       </c>
       <c r="T41" s="27" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="U41" s="21" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="V41" s="21"/>
       <c r="W41" s="27" t="s">
@@ -6163,7 +6163,7 @@
         <v>52.4</v>
       </c>
       <c r="Z41" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA41" s="27"/>
       <c r="AB41"/>
@@ -6253,31 +6253,31 @@
       <c r="M42" s="22"/>
       <c r="N42" s="26"/>
       <c r="O42" s="27" t="s">
-        <v>386</v>
+        <v>359</v>
       </c>
       <c r="P42" s="27" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="Q42" s="27" t="s">
         <v>103</v>
       </c>
       <c r="R42" s="27" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="S42" s="39" t="s">
-        <v>296</v>
+        <v>461</v>
       </c>
       <c r="T42" s="27" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="U42" s="21" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="V42" s="21" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
       <c r="W42" s="27" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="X42" s="27">
         <v>1255</v>
@@ -6345,7 +6345,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>28</v>
@@ -6371,19 +6371,19 @@
       <c r="N43" s="26"/>
       <c r="O43" s="27"/>
       <c r="P43" s="27" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="Q43" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R43" s="27" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="S43" s="39" t="s">
-        <v>301</v>
+        <v>462</v>
       </c>
       <c r="T43" s="27" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="U43" s="21"/>
       <c r="V43" s="21"/>
@@ -6397,7 +6397,7 @@
         <v>114</v>
       </c>
       <c r="Z43" s="27" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="AA43" s="27" t="s">
         <v>114</v>
@@ -6487,22 +6487,22 @@
         <v>551236001639</v>
       </c>
       <c r="O44" s="27" t="s">
-        <v>387</v>
+        <v>360</v>
       </c>
       <c r="P44" s="27" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="Q44" s="27" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="R44" s="27" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="S44" s="39" t="s">
-        <v>307</v>
+        <v>463</v>
       </c>
       <c r="T44" s="27" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="U44" s="21" t="s">
         <v>114</v>
@@ -6518,7 +6518,7 @@
         <v>114</v>
       </c>
       <c r="Z44" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA44" s="27" t="s">
         <v>114</v>
@@ -6577,7 +6577,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="C45" s="22">
         <v>6</v>
@@ -6606,25 +6606,25 @@
         <v>551236002471</v>
       </c>
       <c r="O45" s="27" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
       <c r="P45" s="27" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="Q45" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R45" s="27" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="S45" s="39" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="T45" s="27" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="U45" s="21" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
       <c r="V45" s="21"/>
       <c r="W45" s="27" t="s">
@@ -6637,7 +6637,7 @@
         <v>71</v>
       </c>
       <c r="Z45" s="27" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="AA45" s="27"/>
       <c r="AB45"/>
@@ -6694,7 +6694,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="C46" s="22">
         <v>6</v>
@@ -6723,25 +6723,25 @@
       <c r="M46" s="25"/>
       <c r="N46" s="26"/>
       <c r="O46" s="27" t="s">
-        <v>407</v>
+        <v>380</v>
       </c>
       <c r="P46" s="27" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="Q46" s="27" t="s">
         <v>120</v>
       </c>
       <c r="R46" s="27" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="S46" s="39" t="s">
-        <v>317</v>
+        <v>464</v>
       </c>
       <c r="T46" s="27" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="U46" s="21" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="V46" s="21"/>
       <c r="W46" s="27" t="s">
@@ -6754,7 +6754,7 @@
         <v>42.1</v>
       </c>
       <c r="Z46" s="27" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="AA46" s="27"/>
       <c r="AB46"/>
@@ -6811,7 +6811,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>1</v>
@@ -6846,31 +6846,31 @@
         <v>551236001642</v>
       </c>
       <c r="O47" s="27" t="s">
-        <v>408</v>
+        <v>381</v>
       </c>
       <c r="P47" s="27" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="Q47" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R47" s="27" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="S47" s="39" t="s">
-        <v>323</v>
+        <v>465</v>
       </c>
       <c r="T47" s="27" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="U47" s="21" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="V47" s="21" t="s">
-        <v>456</v>
+        <v>429</v>
       </c>
       <c r="W47" s="27" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="X47" s="27">
         <v>187</v>
@@ -6938,7 +6938,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>1</v>
@@ -6967,25 +6967,25 @@
         <v>551236001644</v>
       </c>
       <c r="O48" s="27" t="s">
-        <v>388</v>
+        <v>361</v>
       </c>
       <c r="P48" s="27" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="Q48" s="27" t="s">
         <v>98</v>
       </c>
       <c r="R48" s="27" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="S48" s="39" t="s">
-        <v>312</v>
+        <v>466</v>
       </c>
       <c r="T48" s="27" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="U48" s="21" t="s">
-        <v>457</v>
+        <v>430</v>
       </c>
       <c r="V48" s="21"/>
       <c r="W48" s="27" t="s">
@@ -6998,7 +6998,7 @@
         <v>84.8</v>
       </c>
       <c r="Z48" s="27" t="s">
-        <v>329</v>
+        <v>304</v>
       </c>
       <c r="AA48" s="27"/>
       <c r="AB48"/>
@@ -7055,7 +7055,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="C49" s="22">
         <v>6</v>
@@ -7086,25 +7086,25 @@
         <v>551236001646</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="P49" s="27" t="s">
-        <v>330</v>
+        <v>305</v>
       </c>
       <c r="Q49" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R49" s="27" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="S49" s="39" t="s">
-        <v>313</v>
+        <v>467</v>
       </c>
       <c r="T49" s="27" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="U49" s="21" t="s">
-        <v>458</v>
+        <v>431</v>
       </c>
       <c r="V49" s="21"/>
       <c r="W49" s="27" t="s">
@@ -7172,7 +7172,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>1</v>
@@ -7199,25 +7199,25 @@
       <c r="M50" s="25"/>
       <c r="N50" s="26"/>
       <c r="O50" s="27" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="P50" s="27" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="Q50" s="27" t="s">
         <v>85</v>
       </c>
       <c r="R50" s="27" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="S50" s="39" t="s">
-        <v>335</v>
+        <v>468</v>
       </c>
       <c r="T50" s="27" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="U50" s="21" t="s">
-        <v>459</v>
+        <v>432</v>
       </c>
       <c r="V50" s="21"/>
       <c r="W50" s="27" t="s">
@@ -7230,7 +7230,7 @@
         <v>77.8</v>
       </c>
       <c r="Z50" s="27" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="AA50" s="27"/>
       <c r="AB50"/>
@@ -7320,31 +7320,31 @@
       </c>
       <c r="N51" s="26"/>
       <c r="O51" s="27" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="P51" s="27" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="Q51" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R51" s="27" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
       <c r="S51" s="39" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="T51" s="27" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="U51" s="21" t="s">
-        <v>464</v>
+        <v>437</v>
       </c>
       <c r="V51" s="21" t="s">
-        <v>465</v>
+        <v>438</v>
       </c>
       <c r="W51" s="27" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="X51" s="27">
         <v>169</v>
@@ -7542,9 +7542,9 @@
     <hyperlink ref="S22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="S23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="S24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="S26" r:id="rId23" display="http://www.rusd.org/park" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="S26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="S27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="S28" r:id="rId25" display="http://www.rusd.org/alternative-education" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="S28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="S25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="S29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="S30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>

</xml_diff>

<commit_message>
fix missing private school data
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CD4AE4-EFDB-6C47-B32A-8719CC13FBFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF07ED4-4867-7540-933B-B65F0DAFBCBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="31020" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="Private" sheetId="14" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All schools'!$A$1:$AA$52</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'All schools'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -2530,10 +2531,10 @@
   </sheetPr>
   <dimension ref="A1:BV52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="S51" sqref="S51"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2957,7 +2958,9 @@
       <c r="L6" s="24">
         <v>441</v>
       </c>
-      <c r="M6" s="25"/>
+      <c r="M6" s="25">
+        <v>1512889</v>
+      </c>
       <c r="N6" s="26"/>
       <c r="O6" s="27" t="s">
         <v>343</v>
@@ -3016,7 +3019,9 @@
         <v>1</v>
       </c>
       <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+      <c r="H7" s="22">
+        <v>1</v>
+      </c>
       <c r="I7" s="22">
         <v>2</v>
       </c>
@@ -3387,7 +3392,9 @@
       <c r="L12" s="24">
         <v>122</v>
       </c>
-      <c r="M12" s="25"/>
+      <c r="M12" s="25" t="s">
+        <v>74</v>
+      </c>
       <c r="N12" s="26"/>
       <c r="O12" s="27" t="s">
         <v>366</v>
@@ -3459,9 +3466,7 @@
       <c r="L13" s="24">
         <v>1711</v>
       </c>
-      <c r="M13" s="25" t="s">
-        <v>74</v>
-      </c>
+      <c r="M13" s="25"/>
       <c r="N13" s="26">
         <v>551236001620</v>
       </c>
@@ -3747,7 +3752,9 @@
       <c r="L17" s="24">
         <v>314</v>
       </c>
-      <c r="M17" s="25"/>
+      <c r="M17" s="25">
+        <v>1507085</v>
+      </c>
       <c r="N17" s="26">
         <v>551236001624</v>
       </c>
@@ -3815,9 +3822,6 @@
       <c r="J18" s="22"/>
       <c r="K18" s="23"/>
       <c r="L18" s="24"/>
-      <c r="M18" s="25">
-        <v>1507085</v>
-      </c>
       <c r="N18" s="26"/>
       <c r="O18" s="27" t="s">
         <v>363</v>
@@ -4167,9 +4171,7 @@
       <c r="L23" s="24">
         <v>2370</v>
       </c>
-      <c r="M23" s="25">
-        <v>1512696</v>
-      </c>
+      <c r="M23" s="25"/>
       <c r="N23" s="26"/>
       <c r="O23" s="27" t="s">
         <v>369</v>
@@ -4313,7 +4315,9 @@
       <c r="L25" s="24">
         <v>150</v>
       </c>
-      <c r="M25" s="25"/>
+      <c r="M25" s="25" t="s">
+        <v>75</v>
+      </c>
       <c r="N25" s="26">
         <v>551236001634</v>
       </c>
@@ -4455,9 +4459,7 @@
       <c r="L27" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="M27" s="25" t="s">
-        <v>75</v>
-      </c>
+      <c r="M27" s="25"/>
       <c r="N27" s="26">
         <v>551236001635</v>
       </c>
@@ -4818,7 +4820,9 @@
       <c r="J30" s="22"/>
       <c r="K30" s="23"/>
       <c r="L30" s="24"/>
-      <c r="M30" s="25"/>
+      <c r="M30" s="25">
+        <v>1512696</v>
+      </c>
       <c r="N30" s="26"/>
       <c r="O30" s="27" t="s">
         <v>374</v>
@@ -5642,7 +5646,9 @@
         <v>1</v>
       </c>
       <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
+      <c r="H37" s="22">
+        <v>1</v>
+      </c>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
       <c r="K37" s="23"/>
@@ -7427,7 +7433,7 @@
       </c>
       <c r="H52" s="22">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I52" s="22">
         <f t="shared" si="1"/>
@@ -7503,7 +7509,7 @@
       <c r="BV52"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A52:AA52 B28:R29 T28:AA29 A1:AA7 B8:AA27 B30:AA51 A8:A51">
+  <conditionalFormatting sqref="A52:AA52 B28:R29 T28:AA29 A1:AA7 B30:AA51 A8:A51 B19:AA27 B18:L18 N18:AA18 B8:AA17">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix bad school ids
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCF217-D409-DF4C-BB6E-231F02BC9CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4027A7A0-AD86-994A-BDF7-81FF23F2105C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26540" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2591,9 +2591,9 @@
   <dimension ref="A1:CA53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3524,7 +3524,7 @@
         <v>4620</v>
       </c>
       <c r="L12" s="24">
-        <v>122</v>
+        <v>1711</v>
       </c>
       <c r="M12" s="25" t="s">
         <v>74</v>
@@ -7167,9 +7167,7 @@
       <c r="M47" s="25">
         <v>1511433</v>
       </c>
-      <c r="N47" s="26">
-        <v>551236001642</v>
-      </c>
+      <c r="N47" s="26"/>
       <c r="O47" s="27" t="s">
         <v>490</v>
       </c>
@@ -7294,7 +7292,7 @@
       </c>
       <c r="M48" s="25"/>
       <c r="N48" s="26">
-        <v>551236001644</v>
+        <v>551236001642</v>
       </c>
       <c r="O48" s="27" t="s">
         <v>352</v>

</xml_diff>

<commit_message>
update db and handle nces/pss grade conversion
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4027A7A0-AD86-994A-BDF7-81FF23F2105C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2009F2-E981-0B41-8686-71BA00D1C054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26540" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2591,9 +2591,9 @@
   <dimension ref="A1:CA53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3501,10 +3501,10 @@
         <v>39</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D12" s="22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="22">
         <v>1</v>
@@ -3602,9 +3602,7 @@
       <c r="K13" s="23">
         <v>4620</v>
       </c>
-      <c r="L13" s="24">
-        <v>1711</v>
-      </c>
+      <c r="L13" s="24"/>
       <c r="M13" s="25"/>
       <c r="N13" s="26">
         <v>551236001620</v>

</xml_diff>

<commit_message>
update and fix the school ids
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2009F2-E981-0B41-8686-71BA00D1C054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1840607D-7A66-A74B-BD26-971D1154E7AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26540" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17620" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All schools" sheetId="13" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="490">
   <si>
     <t>name</t>
   </si>
@@ -967,10 +967,6 @@
   </si>
   <si>
     <t xml:space="preserve">The Prairie School </t>
-  </si>
-  <si>
-    <t>0494
-2317</t>
   </si>
   <si>
     <t>The R.E.A.L. School</t>
@@ -2073,7 +2069,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2214,6 +2210,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2260,7 +2263,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2591,9 +2601,9 @@
   <dimension ref="A1:CA53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2608,7 +2618,7 @@
     <col min="9" max="10" width="8.83203125" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.5" style="12" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="52" customWidth="1"/>
     <col min="14" max="14" width="14.5" style="9" customWidth="1"/>
     <col min="15" max="15" width="15.6640625" style="9" customWidth="1"/>
     <col min="16" max="16" width="20.5" style="9" customWidth="1"/>
@@ -2676,22 +2686,22 @@
         <v>83</v>
       </c>
       <c r="R1" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>463</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>460</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>461</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>464</v>
       </c>
       <c r="V1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="X1" s="38" t="s">
         <v>78</v>
@@ -2757,7 +2767,7 @@
         <v>550004502575</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>97</v>
@@ -2780,7 +2790,7 @@
         <v>101</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="27" t="s">
@@ -2809,7 +2819,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="22">
         <v>1</v>
@@ -2827,10 +2837,12 @@
       <c r="L3" s="24">
         <v>114</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="26"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="26">
+        <v>551236002708</v>
+      </c>
       <c r="O3" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P3" s="27" t="s">
         <v>102</v>
@@ -2847,7 +2859,7 @@
       </c>
       <c r="W3" s="27"/>
       <c r="X3" s="39" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y3" s="27" t="s">
         <v>105</v>
@@ -2903,7 +2915,7 @@
         <v>551236001621</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P4" s="28" t="s">
         <v>84</v>
@@ -2926,7 +2938,7 @@
         <v>88</v>
       </c>
       <c r="Z4" s="47" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AA4" s="21"/>
       <c r="AB4" s="27" t="s">
@@ -2978,7 +2990,7 @@
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
       <c r="O5" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P5" s="27" t="s">
         <v>106</v>
@@ -3001,7 +3013,7 @@
         <v>109</v>
       </c>
       <c r="Z5" s="21" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AA5" s="21"/>
       <c r="AB5" s="27" t="s">
@@ -3057,7 +3069,7 @@
       </c>
       <c r="N6" s="26"/>
       <c r="O6" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P6" s="27" t="s">
         <v>118</v>
@@ -3070,7 +3082,7 @@
       <c r="T6" s="27"/>
       <c r="U6" s="27"/>
       <c r="V6" s="27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="W6" s="27"/>
       <c r="X6" s="39" t="s">
@@ -3136,25 +3148,25 @@
       </c>
       <c r="N7" s="26"/>
       <c r="O7" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P7" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="R7" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="S7" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="T7" s="27" t="s">
         <v>468</v>
       </c>
-      <c r="Q7" s="27" t="s">
-        <v>470</v>
-      </c>
-      <c r="R7" s="27" t="s">
+      <c r="U7" s="27" t="s">
         <v>465</v>
-      </c>
-      <c r="S7" s="27" t="s">
-        <v>467</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>469</v>
-      </c>
-      <c r="U7" s="27" t="s">
-        <v>466</v>
       </c>
       <c r="V7" s="27" t="s">
         <v>124</v>
@@ -3163,13 +3175,13 @@
         <v>124</v>
       </c>
       <c r="X7" s="39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y7" s="27" t="s">
         <v>125</v>
       </c>
       <c r="Z7" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AA7" s="21"/>
       <c r="AB7" s="27" t="s">
@@ -3223,7 +3235,7 @@
         <v>551236001611</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P8" s="27" t="s">
         <v>128</v>
@@ -3246,7 +3258,7 @@
         <v>132</v>
       </c>
       <c r="Z8" s="21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AA8" s="21"/>
       <c r="AB8" s="27" t="s">
@@ -3269,7 +3281,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>1</v>
@@ -3298,7 +3310,7 @@
         <v>551236001614</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="P9" s="27" t="s">
         <v>133</v>
@@ -3321,7 +3333,7 @@
         <v>136</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AA9" s="21"/>
       <c r="AB9" s="27" t="s">
@@ -3344,7 +3356,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>1</v>
@@ -3375,7 +3387,7 @@
         <v>551236002311</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P10" s="27" t="s">
         <v>137</v>
@@ -3398,7 +3410,7 @@
         <v>140</v>
       </c>
       <c r="Z10" s="21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AA10" s="21"/>
       <c r="AB10" s="27" t="s">
@@ -3421,7 +3433,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>25</v>
@@ -3452,7 +3464,7 @@
         <v>551236001608</v>
       </c>
       <c r="O11" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P11" s="27" t="s">
         <v>141</v>
@@ -3475,7 +3487,7 @@
         <v>144</v>
       </c>
       <c r="Z11" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AA11" s="21"/>
       <c r="AB11" s="27" t="s">
@@ -3531,7 +3543,7 @@
       </c>
       <c r="N12" s="26"/>
       <c r="O12" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P12" s="27" t="s">
         <v>146</v>
@@ -3554,10 +3566,10 @@
         <v>150</v>
       </c>
       <c r="Z12" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="AA12" s="21" t="s">
         <v>383</v>
-      </c>
-      <c r="AA12" s="21" t="s">
-        <v>384</v>
       </c>
       <c r="AB12" s="27" t="s">
         <v>151</v>
@@ -3602,13 +3614,15 @@
       <c r="K13" s="23">
         <v>4620</v>
       </c>
-      <c r="L13" s="24"/>
+      <c r="L13" s="50">
+        <v>492</v>
+      </c>
       <c r="M13" s="25"/>
       <c r="N13" s="26">
         <v>551236001620</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P13" s="27" t="s">
         <v>152</v>
@@ -3631,7 +3645,7 @@
         <v>155</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="27" t="s">
@@ -3676,12 +3690,14 @@
         <v>4620</v>
       </c>
       <c r="L14" s="24">
-        <v>492</v>
+        <v>130</v>
       </c>
       <c r="M14" s="25"/>
-      <c r="N14" s="26"/>
+      <c r="N14" s="26">
+        <v>551236001622</v>
+      </c>
       <c r="O14" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P14" s="27" t="s">
         <v>157</v>
@@ -3704,7 +3720,7 @@
         <v>160</v>
       </c>
       <c r="Z14" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AA14" s="21"/>
       <c r="AB14" s="27" t="s">
@@ -3727,7 +3743,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>25</v>
@@ -3749,14 +3765,14 @@
         <v>4620</v>
       </c>
       <c r="L15" s="24">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M15" s="25"/>
       <c r="N15" s="26">
-        <v>551236001622</v>
+        <v>551236001623</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P15" s="27" t="s">
         <v>162</v>
@@ -3779,7 +3795,7 @@
         <v>165</v>
       </c>
       <c r="Z15" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AA15" s="21"/>
       <c r="AB15" s="27" t="s">
@@ -3802,7 +3818,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>1</v>
@@ -3826,14 +3842,13 @@
         <v>4620</v>
       </c>
       <c r="L16" s="24">
-        <v>132</v>
-      </c>
-      <c r="M16" s="25"/>
+        <v>134</v>
+      </c>
       <c r="N16" s="26">
-        <v>551236001623</v>
+        <v>551236001624</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P16" s="27" t="s">
         <v>167</v>
@@ -3856,7 +3871,7 @@
         <v>170</v>
       </c>
       <c r="Z16" s="21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AA16" s="21"/>
       <c r="AB16" s="27" t="s">
@@ -3906,17 +3921,11 @@
       <c r="K17" s="23">
         <v>4620</v>
       </c>
-      <c r="L17" s="24">
-        <v>314</v>
-      </c>
       <c r="M17" s="25">
         <v>1507085</v>
       </c>
-      <c r="N17" s="26">
-        <v>551236001624</v>
-      </c>
       <c r="O17" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P17" s="27" t="s">
         <v>171</v>
@@ -3940,7 +3949,7 @@
       </c>
       <c r="Z17" s="21"/>
       <c r="AA17" s="21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AB17" s="27" t="s">
         <v>175</v>
@@ -3982,11 +3991,18 @@
         <v>1</v>
       </c>
       <c r="J18" s="22"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="N18" s="26"/>
+      <c r="K18" s="23">
+        <v>4620</v>
+      </c>
+      <c r="L18" s="24">
+        <v>136</v>
+      </c>
+      <c r="M18" s="25"/>
+      <c r="N18" s="26">
+        <v>551236001626</v>
+      </c>
       <c r="O18" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P18" s="27" t="s">
         <v>176</v>
@@ -4009,7 +4025,7 @@
         <v>179</v>
       </c>
       <c r="Z18" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AA18" s="21"/>
       <c r="AB18" s="27" t="s">
@@ -4032,7 +4048,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>1</v>
@@ -4054,14 +4070,14 @@
         <v>4620</v>
       </c>
       <c r="L19" s="24">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="M19" s="25"/>
       <c r="N19" s="26">
-        <v>551236001626</v>
+        <v>551236001627</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P19" s="27" t="s">
         <v>180</v>
@@ -4084,7 +4100,7 @@
         <v>183</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="27" t="s">
@@ -4107,7 +4123,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>1</v>
@@ -4129,14 +4145,14 @@
         <v>4620</v>
       </c>
       <c r="L20" s="24">
-        <v>111</v>
+        <v>720</v>
       </c>
       <c r="M20" s="25"/>
       <c r="N20" s="26">
-        <v>551236001627</v>
+        <v>551236003337</v>
       </c>
       <c r="O20" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="P20" s="27" t="s">
         <v>184</v>
@@ -4159,7 +4175,7 @@
         <v>187</v>
       </c>
       <c r="Z20" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AA20" s="21"/>
       <c r="AB20" s="27" t="s">
@@ -4182,7 +4198,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>1</v>
@@ -4204,14 +4220,14 @@
         <v>4620</v>
       </c>
       <c r="L21" s="24">
-        <v>720</v>
+        <v>138</v>
       </c>
       <c r="M21" s="25"/>
       <c r="N21" s="26">
-        <v>551236003337</v>
+        <v>551236001628</v>
       </c>
       <c r="O21" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P21" s="27" t="s">
         <v>189</v>
@@ -4234,7 +4250,7 @@
         <v>192</v>
       </c>
       <c r="Z21" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA21" s="21"/>
       <c r="AB21" s="27" t="s">
@@ -4281,14 +4297,14 @@
         <v>4620</v>
       </c>
       <c r="L22" s="24">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="M22" s="25"/>
       <c r="N22" s="26">
-        <v>551236001628</v>
+        <v>551236001632</v>
       </c>
       <c r="O22" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P22" s="27" t="s">
         <v>193</v>
@@ -4311,7 +4327,7 @@
         <v>196</v>
       </c>
       <c r="Z22" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AA22" s="21"/>
       <c r="AB22" s="27" t="s">
@@ -4356,12 +4372,14 @@
         <v>4620</v>
       </c>
       <c r="L23" s="24">
-        <v>2370</v>
+        <v>150</v>
       </c>
       <c r="M23" s="25"/>
-      <c r="N23" s="26"/>
+      <c r="N23" s="26">
+        <v>551236001634</v>
+      </c>
       <c r="O23" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P23" s="27" t="s">
         <v>198</v>
@@ -4384,7 +4402,7 @@
         <v>201</v>
       </c>
       <c r="Z23" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AA23" s="21"/>
       <c r="AB23" s="27" t="s">
@@ -4425,18 +4443,18 @@
         <v>1</v>
       </c>
       <c r="J24" s="22"/>
-      <c r="K24" s="23">
+      <c r="K24" s="32">
         <v>4620</v>
       </c>
-      <c r="L24" s="24">
-        <v>148</v>
-      </c>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26">
-        <v>551236001632</v>
+      <c r="L24" s="33">
+        <v>112</v>
+      </c>
+      <c r="M24" s="34"/>
+      <c r="N24" s="35">
+        <v>551236001605</v>
       </c>
       <c r="O24" s="27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P24" s="27" t="s">
         <v>202</v>
@@ -4459,7 +4477,7 @@
         <v>205</v>
       </c>
       <c r="Z24" s="21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AA24" s="21"/>
       <c r="AB24" s="27" t="s">
@@ -4506,20 +4524,14 @@
       <c r="J25" s="22">
         <v>2</v>
       </c>
-      <c r="K25" s="23">
-        <v>4620</v>
-      </c>
-      <c r="L25" s="24">
-        <v>150</v>
-      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="24"/>
       <c r="M25" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="N25" s="26">
-        <v>551236001634</v>
-      </c>
+      <c r="N25" s="26"/>
       <c r="O25" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P25" s="27" t="s">
         <v>206</v>
@@ -4536,14 +4548,14 @@
       </c>
       <c r="W25" s="49"/>
       <c r="X25" s="43" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Y25" s="27" t="s">
         <v>208</v>
       </c>
       <c r="Z25" s="21"/>
       <c r="AA25" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AB25" s="27" t="s">
         <v>175</v>
@@ -4589,14 +4601,14 @@
         <v>4620</v>
       </c>
       <c r="L26" s="33">
-        <v>112</v>
+        <v>494</v>
       </c>
       <c r="M26" s="34"/>
       <c r="N26" s="35">
-        <v>551236001605</v>
+        <v>551236001635</v>
       </c>
       <c r="O26" s="36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P26" s="36" t="s">
         <v>210</v>
@@ -4613,13 +4625,13 @@
       </c>
       <c r="W26" s="36"/>
       <c r="X26" s="39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Y26" s="36" t="s">
         <v>212</v>
       </c>
       <c r="Z26" s="30" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AA26" s="30"/>
       <c r="AB26" s="36" t="s">
@@ -4663,15 +4675,11 @@
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="23"/>
-      <c r="L27" s="24" t="s">
-        <v>310</v>
-      </c>
+      <c r="L27" s="24"/>
       <c r="M27" s="25"/>
-      <c r="N27" s="26">
-        <v>551236001635</v>
-      </c>
+      <c r="N27" s="26"/>
       <c r="O27" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P27" s="27" t="s">
         <v>216</v>
@@ -4688,7 +4696,7 @@
       </c>
       <c r="W27" s="27"/>
       <c r="X27" s="39" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y27" s="27" t="s">
         <v>218</v>
@@ -4799,7 +4807,7 @@
         <v>551236003045</v>
       </c>
       <c r="O28" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="P28" s="27" t="s">
         <v>219</v>
@@ -4816,13 +4824,13 @@
       </c>
       <c r="W28" s="49"/>
       <c r="X28" s="44" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Y28" s="27" t="s">
         <v>221</v>
       </c>
       <c r="Z28" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AA28" s="21"/>
       <c r="AB28" s="27" t="s">
@@ -4925,7 +4933,7 @@
       </c>
       <c r="N29" s="26"/>
       <c r="O29" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P29" s="27" t="s">
         <v>223</v>
@@ -4942,14 +4950,14 @@
       </c>
       <c r="W29" s="49"/>
       <c r="X29" s="45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y29" s="27" t="s">
         <v>225</v>
       </c>
       <c r="Z29" s="21"/>
       <c r="AA29" s="21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AB29" s="27" t="s">
         <v>226</v>
@@ -5040,14 +5048,18 @@
         <v>2</v>
       </c>
       <c r="J30" s="22"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="24"/>
+      <c r="K30" s="23">
+        <v>4620</v>
+      </c>
+      <c r="L30" s="24">
+        <v>2370</v>
+      </c>
       <c r="M30" s="25">
         <v>1512696</v>
       </c>
       <c r="N30" s="26"/>
       <c r="O30" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="P30" s="27" t="s">
         <v>227</v>
@@ -5064,16 +5076,16 @@
       </c>
       <c r="W30" s="27"/>
       <c r="X30" s="39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y30" s="27" t="s">
         <v>229</v>
       </c>
       <c r="Z30" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA30" s="21" t="s">
         <v>394</v>
-      </c>
-      <c r="AA30" s="21" t="s">
-        <v>395</v>
       </c>
       <c r="AB30" s="27" t="s">
         <v>230</v>
@@ -5166,14 +5178,18 @@
         <v>0</v>
       </c>
       <c r="J31" s="22"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
+      <c r="K31" s="23">
+        <v>4620</v>
+      </c>
+      <c r="L31" s="24">
+        <v>2372</v>
+      </c>
       <c r="M31" s="25">
         <v>1511295</v>
       </c>
       <c r="N31" s="26"/>
       <c r="O31" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="P31" s="27" t="s">
         <v>231</v>
@@ -5190,7 +5206,7 @@
       </c>
       <c r="W31" s="27"/>
       <c r="X31" s="39" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Y31" s="27" t="s">
         <v>233</v>
@@ -5268,7 +5284,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>1</v>
@@ -5297,7 +5313,7 @@
         <v>551236001636</v>
       </c>
       <c r="O32" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P32" s="27" t="s">
         <v>235</v>
@@ -5314,13 +5330,13 @@
       </c>
       <c r="W32" s="27"/>
       <c r="X32" s="39" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Y32" s="27" t="s">
         <v>237</v>
       </c>
       <c r="Z32" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AA32" s="21"/>
       <c r="AB32" s="27" t="s">
@@ -5421,43 +5437,43 @@
       <c r="M33" s="25"/>
       <c r="N33" s="26"/>
       <c r="O33" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P33" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q33" s="27" t="s">
+        <v>475</v>
+      </c>
+      <c r="R33" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="S33" s="27" t="s">
         <v>474</v>
-      </c>
-      <c r="Q33" s="27" t="s">
-        <v>476</v>
-      </c>
-      <c r="R33" s="27" t="s">
-        <v>472</v>
-      </c>
-      <c r="S33" s="27" t="s">
-        <v>475</v>
       </c>
       <c r="T33" s="27" t="s">
         <v>103</v>
       </c>
       <c r="U33" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="V33" s="27" t="s">
+        <v>476</v>
+      </c>
+      <c r="W33" s="27" t="s">
         <v>477</v>
       </c>
-      <c r="W33" s="27" t="s">
-        <v>478</v>
-      </c>
       <c r="X33" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Y33" s="27" t="s">
         <v>239</v>
       </c>
       <c r="Z33" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="AA33" s="21" t="s">
         <v>405</v>
-      </c>
-      <c r="AA33" s="21" t="s">
-        <v>406</v>
       </c>
       <c r="AB33" s="27" t="s">
         <v>240</v>
@@ -5528,7 +5544,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>1</v>
@@ -5557,7 +5573,7 @@
         <v>551236001637</v>
       </c>
       <c r="O34" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P34" s="27" t="s">
         <v>241</v>
@@ -5574,13 +5590,13 @@
       </c>
       <c r="W34" s="27"/>
       <c r="X34" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Y34" s="27" t="s">
         <v>243</v>
       </c>
       <c r="Z34" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AA34" s="21"/>
       <c r="AB34" s="27" t="s">
@@ -5650,7 +5666,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>1</v>
@@ -5679,7 +5695,7 @@
         <v>551236003044</v>
       </c>
       <c r="O35" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P35" s="27" t="s">
         <v>244</v>
@@ -5696,13 +5712,13 @@
       </c>
       <c r="W35" s="27"/>
       <c r="X35" s="39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Y35" s="27" t="s">
         <v>247</v>
       </c>
       <c r="Z35" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AA35" s="21"/>
       <c r="AB35" s="27" t="s">
@@ -5801,7 +5817,7 @@
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P36" s="27" t="s">
         <v>248</v>
@@ -5818,16 +5834,16 @@
       </c>
       <c r="W36" s="27"/>
       <c r="X36" s="39" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="Y36" s="27" t="s">
         <v>250</v>
       </c>
       <c r="Z36" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="AA36" s="21" t="s">
         <v>421</v>
-      </c>
-      <c r="AA36" s="21" t="s">
-        <v>422</v>
       </c>
       <c r="AB36" s="27" t="s">
         <v>175</v>
@@ -5918,14 +5934,18 @@
       </c>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
+      <c r="K37" s="23">
+        <v>4620</v>
+      </c>
+      <c r="L37" s="23">
+        <v>4910</v>
+      </c>
       <c r="M37" s="25">
         <v>1511444</v>
       </c>
       <c r="N37" s="26"/>
       <c r="O37" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P37" s="27" t="s">
         <v>253</v>
@@ -5942,7 +5962,7 @@
       </c>
       <c r="W37" s="27"/>
       <c r="X37" s="39" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="Y37" s="27" t="s">
         <v>255</v>
@@ -6047,7 +6067,7 @@
       <c r="M38" s="25"/>
       <c r="N38" s="26"/>
       <c r="O38" s="27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="P38" s="27" t="s">
         <v>257</v>
@@ -6064,16 +6084,16 @@
       </c>
       <c r="W38" s="27"/>
       <c r="X38" s="39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Y38" s="27" t="s">
         <v>259</v>
       </c>
       <c r="Z38" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="AA38" s="21" t="s">
         <v>408</v>
-      </c>
-      <c r="AA38" s="21" t="s">
-        <v>409</v>
       </c>
       <c r="AB38" s="27" t="s">
         <v>175</v>
@@ -6144,7 +6164,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>28</v>
@@ -6173,7 +6193,7 @@
       </c>
       <c r="N39" s="26"/>
       <c r="O39" s="27" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P39" s="27" t="s">
         <v>263</v>
@@ -6190,16 +6210,16 @@
       </c>
       <c r="W39" s="27"/>
       <c r="X39" s="39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Y39" s="27" t="s">
         <v>265</v>
       </c>
       <c r="Z39" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="AA39" s="21" t="s">
         <v>423</v>
-      </c>
-      <c r="AA39" s="21" t="s">
-        <v>424</v>
       </c>
       <c r="AB39" s="27" t="s">
         <v>175</v>
@@ -6270,7 +6290,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>25</v>
@@ -6299,7 +6319,7 @@
       </c>
       <c r="N40" s="26"/>
       <c r="O40" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>266</v>
@@ -6316,16 +6336,16 @@
       </c>
       <c r="W40" s="27"/>
       <c r="X40" s="39" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Y40" s="27" t="s">
         <v>268</v>
       </c>
       <c r="Z40" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="AA40" s="21" t="s">
         <v>410</v>
-      </c>
-      <c r="AA40" s="21" t="s">
-        <v>411</v>
       </c>
       <c r="AB40" s="27" t="s">
         <v>175</v>
@@ -6396,7 +6416,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>1</v>
@@ -6425,7 +6445,7 @@
         <v>551236001638</v>
       </c>
       <c r="O41" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="P41" s="27" t="s">
         <v>269</v>
@@ -6442,13 +6462,13 @@
       </c>
       <c r="W41" s="27"/>
       <c r="X41" s="39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Y41" s="27" t="s">
         <v>271</v>
       </c>
       <c r="Z41" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AA41" s="21"/>
       <c r="AB41" s="27" t="s">
@@ -6548,10 +6568,10 @@
       <c r="L42" s="23">
         <v>3430</v>
       </c>
-      <c r="M42" s="22"/>
+      <c r="M42" s="51"/>
       <c r="N42" s="26"/>
       <c r="O42" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P42" s="27" t="s">
         <v>272</v>
@@ -6568,16 +6588,16 @@
       </c>
       <c r="W42" s="27"/>
       <c r="X42" s="39" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Y42" s="27" t="s">
         <v>273</v>
       </c>
       <c r="Z42" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA42" s="21" t="s">
         <v>413</v>
-      </c>
-      <c r="AA42" s="21" t="s">
-        <v>414</v>
       </c>
       <c r="AB42" s="27" t="s">
         <v>274</v>
@@ -6648,7 +6668,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>28</v>
@@ -6688,7 +6708,7 @@
       </c>
       <c r="W43" s="27"/>
       <c r="X43" s="39" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y43" s="27" t="s">
         <v>277</v>
@@ -6791,11 +6811,9 @@
         <v>1750</v>
       </c>
       <c r="M44" s="25"/>
-      <c r="N44" s="26">
-        <v>551236001639</v>
-      </c>
+      <c r="N44" s="26"/>
       <c r="O44" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P44" s="27" t="s">
         <v>279</v>
@@ -6812,7 +6830,7 @@
       </c>
       <c r="W44" s="27"/>
       <c r="X44" s="39" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y44" s="27" t="s">
         <v>282</v>
@@ -6890,7 +6908,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C45" s="22">
         <v>6</v>
@@ -6916,10 +6934,10 @@
       </c>
       <c r="M45" s="25"/>
       <c r="N45" s="26">
-        <v>551236002471</v>
+        <v>551236001639</v>
       </c>
       <c r="O45" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P45" s="27" t="s">
         <v>283</v>
@@ -6936,13 +6954,13 @@
       </c>
       <c r="W45" s="27"/>
       <c r="X45" s="39" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="Y45" s="27" t="s">
         <v>285</v>
       </c>
       <c r="Z45" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AA45" s="21"/>
       <c r="AB45" s="27" t="s">
@@ -7012,7 +7030,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C46" s="22">
         <v>6</v>
@@ -7039,9 +7057,11 @@
         <v>800</v>
       </c>
       <c r="M46" s="25"/>
-      <c r="N46" s="26"/>
+      <c r="N46" s="26">
+        <v>551236002471</v>
+      </c>
       <c r="O46" s="27" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P46" s="27" t="s">
         <v>290</v>
@@ -7058,13 +7078,13 @@
       </c>
       <c r="W46" s="27"/>
       <c r="X46" s="39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Y46" s="27" t="s">
         <v>288</v>
       </c>
       <c r="Z46" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AA46" s="21"/>
       <c r="AB46" s="27" t="s">
@@ -7134,7 +7154,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>1</v>
@@ -7167,7 +7187,7 @@
       </c>
       <c r="N47" s="26"/>
       <c r="O47" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="P47" s="27" t="s">
         <v>291</v>
@@ -7184,16 +7204,16 @@
       </c>
       <c r="W47" s="27"/>
       <c r="X47" s="39" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Y47" s="27" t="s">
         <v>293</v>
       </c>
       <c r="Z47" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="AA47" s="21" t="s">
         <v>416</v>
-      </c>
-      <c r="AA47" s="21" t="s">
-        <v>417</v>
       </c>
       <c r="AB47" s="27" t="s">
         <v>294</v>
@@ -7264,7 +7284,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>1</v>
@@ -7293,7 +7313,7 @@
         <v>551236001642</v>
       </c>
       <c r="O48" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P48" s="27" t="s">
         <v>295</v>
@@ -7310,13 +7330,13 @@
       </c>
       <c r="W48" s="27"/>
       <c r="X48" s="39" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Y48" s="27" t="s">
         <v>297</v>
       </c>
       <c r="Z48" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AA48" s="21"/>
       <c r="AB48" s="27" t="s">
@@ -7386,7 +7406,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C49" s="22">
         <v>6</v>
@@ -7414,10 +7434,10 @@
       </c>
       <c r="M49" s="25"/>
       <c r="N49" s="26">
-        <v>551236001646</v>
+        <v>551236001644</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P49" s="27" t="s">
         <v>299</v>
@@ -7434,13 +7454,13 @@
       </c>
       <c r="W49" s="27"/>
       <c r="X49" s="39" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="Y49" s="27" t="s">
         <v>301</v>
       </c>
       <c r="Z49" s="21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AA49" s="21"/>
       <c r="AB49" s="27" t="s">
@@ -7508,7 +7528,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>1</v>
@@ -7533,9 +7553,11 @@
         <v>164</v>
       </c>
       <c r="M50" s="25"/>
-      <c r="N50" s="26"/>
+      <c r="N50" s="26">
+        <v>551236001646</v>
+      </c>
       <c r="O50" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P50" s="27" t="s">
         <v>302</v>
@@ -7552,13 +7574,13 @@
       </c>
       <c r="W50" s="27"/>
       <c r="X50" s="39" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Y50" s="27" t="s">
         <v>304</v>
       </c>
       <c r="Z50" s="21" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AA50" s="21"/>
       <c r="AB50" s="27" t="s">
@@ -7661,7 +7683,7 @@
       </c>
       <c r="N51" s="26"/>
       <c r="O51" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="P51" s="27" t="s">
         <v>305</v>
@@ -7678,19 +7700,19 @@
       </c>
       <c r="W51" s="27"/>
       <c r="X51" s="39" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y51" s="27" t="s">
         <v>307</v>
       </c>
       <c r="Z51" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="AA51" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="AA51" s="21" t="s">
-        <v>426</v>
-      </c>
       <c r="AB51" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AC51" s="27">
         <v>169</v>
@@ -7755,7 +7777,7 @@
     <row r="52" spans="1:79" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="46"/>
       <c r="B52" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>1</v>
@@ -7778,34 +7800,38 @@
       <c r="K52" s="23">
         <v>4620</v>
       </c>
-      <c r="L52" s="24"/>
-      <c r="M52" s="25"/>
+      <c r="L52" s="24">
+        <v>8505</v>
+      </c>
+      <c r="M52" s="25">
+        <v>1512619</v>
+      </c>
       <c r="N52" s="26"/>
       <c r="O52" s="27"/>
       <c r="P52" s="27" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q52" s="27" t="s">
         <v>480</v>
-      </c>
-      <c r="Q52" s="27" t="s">
-        <v>481</v>
       </c>
       <c r="R52" s="27"/>
       <c r="S52" s="27"/>
       <c r="T52" s="27"/>
       <c r="U52" s="27"/>
       <c r="V52" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="W52" s="27"/>
       <c r="X52" s="39" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Y52" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Z52" s="21"/>
       <c r="AA52" s="21"/>
       <c r="AB52" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AC52" s="27">
         <v>93</v>
@@ -7814,7 +7840,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="AE52" s="27" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AF52" s="27">
         <v>48.9</v>
@@ -7900,7 +7926,7 @@
       </c>
       <c r="K53" s="23"/>
       <c r="L53" s="23"/>
-      <c r="M53" s="27"/>
+      <c r="M53" s="25"/>
       <c r="N53" s="27"/>
       <c r="O53" s="27"/>
       <c r="P53" s="27"/>
@@ -7969,20 +7995,31 @@
       <c r="CA53"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A53:AF53 B28:W29 Y28:AF29 A1:AF7 B30:AF52 A8:A52 B19:AF27 B18:L18 N18:AF18 B8:AF17">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A53:AF53 B28:W29 Y28:AF29 A1:AF7 A8:A52 B8:AF15 B17:K17 B16:L16 M17 O17:AF17 N16:AF16 B25:AF27 B24:J24 O24:AF24 B18:AF23 B30:AF52">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" priority="3">
+    <cfRule type="expression" priority="9">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" priority="4">
+    <cfRule type="expression" priority="10">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24:N24">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="2">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="3">
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -9223,7 +9260,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:J42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J42">
     <sortCondition ref="E2:E42"/>
   </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10728,7 +10765,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J12">
     <sortCondition ref="G2:G12"/>
   </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12319,7 +12356,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J22">
     <sortCondition ref="H2:H22"/>
   </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove extra paren in bull
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F66CA3-93B2-3C42-ACEA-A6DD33F07C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF7E03-E926-B948-A74E-35E5F64184C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,9 +384,6 @@
     <t>Not available</t>
   </si>
   <si>
-    <t>Kindergarten readiness, special education, Dual-language, Parent-Child Oriented Classroom ((P-COC)</t>
-  </si>
-  <si>
     <t>Private, Independent</t>
   </si>
   <si>
@@ -1518,6 +1515,9 @@
   </si>
   <si>
     <t>http://www.wisconsinlutheranschool.org</t>
+  </si>
+  <si>
+    <t>Kindergarten readiness, special education, Dual-language, Parent-Child Oriented Classroom (P-COC)</t>
   </si>
 </sst>
 </file>
@@ -2621,10 +2621,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2707,22 +2707,22 @@
         <v>83</v>
       </c>
       <c r="R1" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>459</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>456</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>457</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>460</v>
       </c>
       <c r="V1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="X1" s="38" t="s">
         <v>78</v>
@@ -2788,7 +2788,7 @@
         <v>550004502575</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>97</v>
@@ -2811,7 +2811,7 @@
         <v>101</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="27" t="s">
@@ -2863,7 +2863,7 @@
         <v>551236002708</v>
       </c>
       <c r="O3" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P3" s="27" t="s">
         <v>102</v>
@@ -2880,7 +2880,7 @@
       </c>
       <c r="W3" s="27"/>
       <c r="X3" s="39" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Y3" s="27" t="s">
         <v>105</v>
@@ -2897,7 +2897,7 @@
         <v>114</v>
       </c>
       <c r="AE3" s="27" t="s">
-        <v>115</v>
+        <v>491</v>
       </c>
       <c r="AF3" s="27"/>
     </row>
@@ -2936,7 +2936,7 @@
       <c r="M4" s="25"/>
       <c r="N4" s="26"/>
       <c r="O4" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P4" s="27" t="s">
         <v>106</v>
@@ -2959,11 +2959,11 @@
         <v>109</v>
       </c>
       <c r="Z4" s="54" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AA4" s="21"/>
       <c r="AB4" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC4" s="27">
         <v>3</v>
@@ -2972,7 +2972,7 @@
         <v>100</v>
       </c>
       <c r="AE4" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AF4" s="27"/>
     </row>
@@ -3015,32 +3015,32 @@
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P5" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q5" s="27" t="s">
         <v>118</v>
-      </c>
-      <c r="Q5" s="27" t="s">
-        <v>119</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="27"/>
       <c r="U5" s="27"/>
       <c r="V5" s="27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="W5" s="27"/>
       <c r="X5" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y5" s="27" t="s">
         <v>120</v>
-      </c>
-      <c r="Y5" s="27" t="s">
-        <v>121</v>
       </c>
       <c r="Z5" s="21"/>
       <c r="AA5" s="21"/>
       <c r="AB5" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC5" s="27">
         <v>180</v>
@@ -3049,7 +3049,7 @@
         <v>41.7</v>
       </c>
       <c r="AE5" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF5" s="27">
         <v>58.8</v>
@@ -3061,7 +3061,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>1</v>
@@ -3090,10 +3090,10 @@
         <v>551236001627</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q6" s="27" t="s">
         <v>103</v>
@@ -3103,17 +3103,17 @@
       <c r="T6" s="27"/>
       <c r="U6" s="27"/>
       <c r="V6" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="W6" s="27"/>
       <c r="X6" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y6" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="Y6" s="27" t="s">
-        <v>183</v>
-      </c>
       <c r="Z6" s="21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AA6" s="21"/>
       <c r="AB6" s="27" t="s">
@@ -3126,7 +3126,7 @@
         <v>81.099999999999994</v>
       </c>
       <c r="AE6" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF6" s="27"/>
     </row>
@@ -3169,44 +3169,44 @@
       </c>
       <c r="N7" s="26"/>
       <c r="O7" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P7" s="27" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="R7" s="27" t="s">
+        <v>460</v>
+      </c>
+      <c r="S7" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="T7" s="27" t="s">
         <v>464</v>
       </c>
-      <c r="Q7" s="27" t="s">
-        <v>466</v>
-      </c>
-      <c r="R7" s="27" t="s">
+      <c r="U7" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="S7" s="27" t="s">
-        <v>463</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>465</v>
-      </c>
-      <c r="U7" s="27" t="s">
-        <v>462</v>
-      </c>
       <c r="V7" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="W7" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="X7" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="Y7" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="W7" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="X7" s="39" t="s">
-        <v>428</v>
-      </c>
-      <c r="Y7" s="27" t="s">
-        <v>125</v>
-      </c>
       <c r="Z7" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AA7" s="21"/>
       <c r="AB7" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC7" s="27">
         <v>351</v>
@@ -3215,7 +3215,7 @@
         <v>76.599999999999994</v>
       </c>
       <c r="AE7" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF7" s="27">
         <v>98</v>
@@ -3256,30 +3256,30 @@
         <v>551236001611</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q8" s="27" t="s">
         <v>128</v>
-      </c>
-      <c r="Q8" s="27" t="s">
-        <v>129</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="27"/>
       <c r="U8" s="27"/>
       <c r="V8" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W8" s="27"/>
       <c r="X8" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y8" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="Y8" s="27" t="s">
-        <v>132</v>
-      </c>
       <c r="Z8" s="21" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AA8" s="21"/>
       <c r="AB8" s="27" t="s">
@@ -3292,7 +3292,7 @@
         <v>81.7</v>
       </c>
       <c r="AE8" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF8" s="27"/>
     </row>
@@ -3302,7 +3302,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>1</v>
@@ -3333,10 +3333,10 @@
         <v>551236002311</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P9" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q9" s="27" t="s">
         <v>85</v>
@@ -3346,17 +3346,17 @@
       <c r="T9" s="27"/>
       <c r="U9" s="27"/>
       <c r="V9" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="W9" s="27"/>
       <c r="X9" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y9" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="Y9" s="27" t="s">
-        <v>140</v>
-      </c>
       <c r="Z9" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AA9" s="21"/>
       <c r="AB9" s="27" t="s">
@@ -3369,7 +3369,7 @@
         <v>28.9</v>
       </c>
       <c r="AE9" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF9" s="27"/>
     </row>
@@ -3379,7 +3379,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>25</v>
@@ -3410,10 +3410,10 @@
         <v>551236001608</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P10" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q10" s="27" t="s">
         <v>98</v>
@@ -3423,17 +3423,17 @@
       <c r="T10" s="27"/>
       <c r="U10" s="27"/>
       <c r="V10" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="W10" s="27"/>
       <c r="X10" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y10" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="Y10" s="27" t="s">
-        <v>144</v>
-      </c>
       <c r="Z10" s="21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AA10" s="21"/>
       <c r="AB10" s="27" t="s">
@@ -3446,7 +3446,7 @@
         <v>57</v>
       </c>
       <c r="AE10" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF10" s="27"/>
     </row>
@@ -3489,36 +3489,36 @@
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P11" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q11" s="27" t="s">
         <v>146</v>
-      </c>
-      <c r="Q11" s="27" t="s">
-        <v>147</v>
       </c>
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="27"/>
       <c r="U11" s="27"/>
       <c r="V11" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W11" s="27"/>
       <c r="X11" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y11" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="Y11" s="27" t="s">
+      <c r="Z11" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="AA11" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="AB11" s="27" t="s">
         <v>150</v>
-      </c>
-      <c r="Z11" s="21" t="s">
-        <v>380</v>
-      </c>
-      <c r="AA11" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="AB11" s="27" t="s">
-        <v>151</v>
       </c>
       <c r="AC11" s="27">
         <v>319</v>
@@ -3527,7 +3527,7 @@
         <v>84.6</v>
       </c>
       <c r="AE11" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF11" s="27">
         <v>99.7</v>
@@ -3568,10 +3568,10 @@
         <v>551236001620</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="P12" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q12" s="27" t="s">
         <v>98</v>
@@ -3581,17 +3581,17 @@
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
       <c r="V12" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W12" s="27"/>
       <c r="X12" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y12" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="Y12" s="27" t="s">
-        <v>155</v>
-      </c>
       <c r="Z12" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AA12" s="21"/>
       <c r="AB12" s="27" t="s">
@@ -3604,7 +3604,7 @@
         <v>63.5</v>
       </c>
       <c r="AE12" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF12" s="27"/>
     </row>
@@ -3643,7 +3643,7 @@
         <v>551236001621</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P13" s="28" t="s">
         <v>84</v>
@@ -3666,7 +3666,7 @@
         <v>88</v>
       </c>
       <c r="Z13" s="55" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="27" t="s">
@@ -3718,30 +3718,30 @@
         <v>551236001622</v>
       </c>
       <c r="O14" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P14" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
       <c r="T14" s="27"/>
       <c r="U14" s="27"/>
       <c r="V14" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W14" s="27"/>
       <c r="X14" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y14" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="Y14" s="27" t="s">
-        <v>160</v>
-      </c>
       <c r="Z14" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AA14" s="21"/>
       <c r="AB14" s="27" t="s">
@@ -3754,7 +3754,7 @@
         <v>93.9</v>
       </c>
       <c r="AE14" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AF14" s="27"/>
     </row>
@@ -3764,7 +3764,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>1</v>
@@ -3793,10 +3793,10 @@
         <v>551236001623</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P15" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q15" s="27" t="s">
         <v>98</v>
@@ -3806,17 +3806,17 @@
       <c r="T15" s="27"/>
       <c r="U15" s="27"/>
       <c r="V15" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W15" s="27"/>
       <c r="X15" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y15" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="Y15" s="27" t="s">
-        <v>165</v>
-      </c>
       <c r="Z15" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AA15" s="21"/>
       <c r="AB15" s="27" t="s">
@@ -3829,7 +3829,7 @@
         <v>41.2</v>
       </c>
       <c r="AE15" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AF15" s="27"/>
     </row>
@@ -3839,7 +3839,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>1</v>
@@ -3870,30 +3870,30 @@
         <v>551236001624</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P16" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q16" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R16" s="27"/>
       <c r="S16" s="27"/>
       <c r="T16" s="27"/>
       <c r="U16" s="27"/>
       <c r="V16" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W16" s="27"/>
       <c r="X16" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Y16" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Z16" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AA16" s="21"/>
       <c r="AB16" s="27" t="s">
@@ -3906,7 +3906,7 @@
         <v>77.3</v>
       </c>
       <c r="AE16" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF16" s="27"/>
     </row>
@@ -3945,10 +3945,10 @@
         <v>1507085</v>
       </c>
       <c r="O17" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P17" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q17" s="27" t="s">
         <v>98</v>
@@ -3958,33 +3958,33 @@
       <c r="T17" s="27"/>
       <c r="U17" s="27"/>
       <c r="V17" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W17" s="27"/>
       <c r="X17" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y17" s="27" t="s">
         <v>173</v>
-      </c>
-      <c r="Y17" s="27" t="s">
-        <v>174</v>
       </c>
       <c r="Z17" s="21"/>
       <c r="AA17" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AB17" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AC17" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD17" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="AD17" s="21" t="s">
-        <v>215</v>
-      </c>
       <c r="AE17" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF17" s="27" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="18" spans="1:79" ht="80" x14ac:dyDescent="0.2">
@@ -3993,7 +3993,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>1</v>
@@ -4022,10 +4022,10 @@
         <v>551236003337</v>
       </c>
       <c r="O18" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P18" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q18" s="27" t="s">
         <v>98</v>
@@ -4035,17 +4035,17 @@
       <c r="T18" s="27"/>
       <c r="U18" s="27"/>
       <c r="V18" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="W18" s="27"/>
       <c r="X18" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y18" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="Y18" s="27" t="s">
-        <v>187</v>
-      </c>
       <c r="Z18" s="21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AA18" s="21"/>
       <c r="AB18" s="27" t="s">
@@ -4058,7 +4058,7 @@
         <v>94.3</v>
       </c>
       <c r="AE18" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AF18" s="27"/>
     </row>
@@ -4068,7 +4068,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>1</v>
@@ -4097,30 +4097,30 @@
         <v>551236001628</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P19" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="27"/>
       <c r="U19" s="27"/>
       <c r="V19" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="W19" s="27"/>
       <c r="X19" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y19" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="Y19" s="27" t="s">
-        <v>192</v>
-      </c>
       <c r="Z19" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="27" t="s">
@@ -4133,7 +4133,7 @@
         <v>87.8</v>
       </c>
       <c r="AE19" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AF19" s="27"/>
     </row>
@@ -4174,10 +4174,10 @@
         <v>551236001632</v>
       </c>
       <c r="O20" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P20" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q20" s="27" t="s">
         <v>103</v>
@@ -4187,17 +4187,17 @@
       <c r="T20" s="27"/>
       <c r="U20" s="27"/>
       <c r="V20" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W20" s="27"/>
       <c r="X20" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y20" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="Y20" s="27" t="s">
-        <v>196</v>
-      </c>
       <c r="Z20" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA20" s="21"/>
       <c r="AB20" s="27" t="s">
@@ -4210,7 +4210,7 @@
         <v>80.8</v>
       </c>
       <c r="AE20" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AF20" s="27"/>
     </row>
@@ -4249,30 +4249,30 @@
         <v>551236001634</v>
       </c>
       <c r="O21" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P21" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q21" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="27"/>
       <c r="U21" s="27"/>
       <c r="V21" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W21" s="27"/>
       <c r="X21" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y21" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="Y21" s="27" t="s">
-        <v>201</v>
-      </c>
       <c r="Z21" s="21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AA21" s="21"/>
       <c r="AB21" s="27" t="s">
@@ -4285,7 +4285,7 @@
         <v>77.7</v>
       </c>
       <c r="AE21" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF21" s="27"/>
     </row>
@@ -4324,30 +4324,30 @@
         <v>551236001605</v>
       </c>
       <c r="O22" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P22" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q22" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R22" s="27"/>
       <c r="S22" s="27"/>
       <c r="T22" s="27"/>
       <c r="U22" s="27"/>
       <c r="V22" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="W22" s="27"/>
       <c r="X22" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y22" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="Y22" s="27" t="s">
-        <v>205</v>
-      </c>
       <c r="Z22" s="21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AA22" s="21"/>
       <c r="AB22" s="27" t="s">
@@ -4360,7 +4360,7 @@
         <v>42.1</v>
       </c>
       <c r="AE22" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF22" s="27"/>
     </row>
@@ -4401,43 +4401,43 @@
       </c>
       <c r="N23" s="26"/>
       <c r="O23" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P23" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q23" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="27"/>
       <c r="U23" s="27"/>
       <c r="V23" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W23" s="27"/>
       <c r="X23" s="51" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Y23" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z23" s="21"/>
       <c r="AA23" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AB23" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AC23" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD23" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE23" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF23" s="27">
         <v>90.5</v>
@@ -4478,10 +4478,10 @@
         <v>551236001635</v>
       </c>
       <c r="O24" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P24" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q24" s="27" t="s">
         <v>103</v>
@@ -4491,17 +4491,17 @@
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="W24" s="27"/>
       <c r="X24" s="39" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Y24" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Z24" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AA24" s="21"/>
       <c r="AB24" s="27" t="s">
@@ -4514,7 +4514,7 @@
         <v>71.900000000000006</v>
       </c>
       <c r="AE24" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF24" s="27"/>
     </row>
@@ -4557,10 +4557,10 @@
         <v>551236003045</v>
       </c>
       <c r="O25" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P25" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q25" s="27" t="s">
         <v>98</v>
@@ -4570,17 +4570,17 @@
       <c r="T25" s="27"/>
       <c r="U25" s="27"/>
       <c r="V25" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W25" s="46"/>
       <c r="X25" s="43" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Y25" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z25" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AA25" s="21"/>
       <c r="AB25" s="27" t="s">
@@ -4593,7 +4593,7 @@
         <v>81.7</v>
       </c>
       <c r="AE25" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF25" s="27"/>
     </row>
@@ -4636,34 +4636,34 @@
       </c>
       <c r="N26" s="35"/>
       <c r="O26" s="36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P26" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q26" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R26" s="36"/>
       <c r="S26" s="36"/>
       <c r="T26" s="36"/>
       <c r="U26" s="36"/>
       <c r="V26" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="W26" s="36"/>
       <c r="X26" s="53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Y26" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z26" s="30"/>
       <c r="AA26" s="30" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AB26" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC26" s="36">
         <v>135</v>
@@ -4672,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="AE26" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF26" s="36">
         <v>45.2</v>
@@ -4715,36 +4715,36 @@
       </c>
       <c r="N27" s="26"/>
       <c r="O27" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P27" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q27" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R27" s="27"/>
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
       <c r="U27" s="27"/>
       <c r="V27" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="W27" s="27"/>
       <c r="X27" s="39" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y27" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z27" s="21" t="s">
+        <v>390</v>
+      </c>
+      <c r="AA27" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="AB27" s="27" t="s">
         <v>229</v>
-      </c>
-      <c r="Z27" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="AA27" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="AB27" s="27" t="s">
-        <v>230</v>
       </c>
       <c r="AC27" s="27">
         <v>264</v>
@@ -4753,7 +4753,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="AE27" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF27" s="27">
         <v>61.7</v>
@@ -4845,34 +4845,34 @@
       </c>
       <c r="N28" s="26"/>
       <c r="O28" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P28" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q28" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
       <c r="U28" s="27"/>
       <c r="V28" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="W28" s="46"/>
       <c r="X28" s="52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Y28" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Z28" s="21" t="s">
         <v>113</v>
       </c>
       <c r="AA28" s="21"/>
       <c r="AB28" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC28" s="27" t="s">
         <v>113</v>
@@ -4881,7 +4881,7 @@
         <v>113</v>
       </c>
       <c r="AE28" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF28" s="27" t="s">
         <v>113</v>
@@ -4940,7 +4940,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>1</v>
@@ -4969,30 +4969,30 @@
         <v>551236001636</v>
       </c>
       <c r="O29" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="P29" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q29" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R29" s="27"/>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
       <c r="U29" s="27"/>
       <c r="V29" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="W29" s="46"/>
       <c r="X29" s="52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y29" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z29" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AA29" s="21"/>
       <c r="AB29" s="27" t="s">
@@ -5005,7 +5005,7 @@
         <v>52.1</v>
       </c>
       <c r="AE29" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AF29" s="27"/>
       <c r="AG29"/>
@@ -5091,50 +5091,50 @@
         <v>1619</v>
       </c>
       <c r="M30" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N30" s="26"/>
       <c r="O30" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P30" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q30" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="R30" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="S30" s="27" t="s">
         <v>470</v>
-      </c>
-      <c r="Q30" s="27" t="s">
-        <v>472</v>
-      </c>
-      <c r="R30" s="27" t="s">
-        <v>468</v>
-      </c>
-      <c r="S30" s="27" t="s">
-        <v>471</v>
       </c>
       <c r="T30" s="27" t="s">
         <v>103</v>
       </c>
       <c r="U30" s="27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="V30" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="W30" s="27" t="s">
         <v>473</v>
       </c>
-      <c r="W30" s="27" t="s">
-        <v>474</v>
-      </c>
       <c r="X30" s="45" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y30" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z30" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA30" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="AB30" s="27" t="s">
         <v>238</v>
-      </c>
-      <c r="Z30" s="21" t="s">
-        <v>402</v>
-      </c>
-      <c r="AA30" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="AB30" s="27" t="s">
-        <v>239</v>
       </c>
       <c r="AC30" s="27">
         <v>356</v>
@@ -5143,7 +5143,7 @@
         <v>84.3</v>
       </c>
       <c r="AE30" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF30" s="27">
         <v>96.9</v>
@@ -5202,7 +5202,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>1</v>
@@ -5231,30 +5231,30 @@
         <v>551236001637</v>
       </c>
       <c r="O31" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P31" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q31" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R31" s="27"/>
       <c r="S31" s="27"/>
       <c r="T31" s="27"/>
       <c r="U31" s="27"/>
       <c r="V31" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W31" s="27"/>
       <c r="X31" s="39" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Y31" s="27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Z31" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AA31" s="21"/>
       <c r="AB31" s="27" t="s">
@@ -5267,7 +5267,7 @@
         <v>87.4</v>
       </c>
       <c r="AE31" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF31" s="27"/>
       <c r="AG31"/>
@@ -5324,7 +5324,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>1</v>
@@ -5353,30 +5353,30 @@
         <v>551236003044</v>
       </c>
       <c r="O32" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P32" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q32" s="27" t="s">
         <v>243</v>
-      </c>
-      <c r="Q32" s="27" t="s">
-        <v>244</v>
       </c>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
       <c r="T32" s="27"/>
       <c r="U32" s="27"/>
       <c r="V32" s="27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W32" s="27"/>
       <c r="X32" s="39" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Y32" s="27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Z32" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AA32" s="21"/>
       <c r="AB32" s="27" t="s">
@@ -5389,7 +5389,7 @@
         <v>86.9</v>
       </c>
       <c r="AE32" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF32" s="27"/>
       <c r="AG32"/>
@@ -5446,7 +5446,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>1</v>
@@ -5475,30 +5475,30 @@
         <v>551236001626</v>
       </c>
       <c r="O33" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P33" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q33" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R33" s="27"/>
       <c r="S33" s="27"/>
       <c r="T33" s="27"/>
       <c r="U33" s="27"/>
       <c r="V33" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W33" s="27"/>
       <c r="X33" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y33" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="Y33" s="27" t="s">
-        <v>179</v>
-      </c>
       <c r="Z33" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AA33" s="21"/>
       <c r="AB33" s="27" t="s">
@@ -5511,7 +5511,7 @@
         <v>85.2</v>
       </c>
       <c r="AE33" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF33" s="27"/>
       <c r="AG33"/>
@@ -5597,48 +5597,48 @@
       </c>
       <c r="N34" s="26"/>
       <c r="O34" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P34" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q34" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
       <c r="T34" s="27"/>
       <c r="U34" s="27"/>
       <c r="V34" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="W34" s="27"/>
       <c r="X34" s="39" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Y34" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z34" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="AA34" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="AB34" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC34" s="27" t="s">
         <v>249</v>
-      </c>
-      <c r="Z34" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="AA34" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="AB34" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="AC34" s="27" t="s">
-        <v>250</v>
       </c>
       <c r="AD34" s="21">
         <v>51.9</v>
       </c>
       <c r="AE34" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF34" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AG34"/>
       <c r="AH34"/>
@@ -5727,32 +5727,32 @@
       </c>
       <c r="N35" s="26"/>
       <c r="O35" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P35" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q35" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R35" s="27"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
       <c r="U35" s="27"/>
       <c r="V35" s="27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W35" s="27"/>
       <c r="X35" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Y35" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z35" s="21"/>
       <c r="AA35" s="21"/>
       <c r="AB35" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AC35" s="27">
         <v>222</v>
@@ -5761,7 +5761,7 @@
         <v>24.3</v>
       </c>
       <c r="AE35" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF35" s="27">
         <v>72.7</v>
@@ -5849,48 +5849,48 @@
       <c r="M36" s="25"/>
       <c r="N36" s="26"/>
       <c r="O36" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P36" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q36" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R36" s="27"/>
       <c r="S36" s="27"/>
       <c r="T36" s="27"/>
       <c r="U36" s="27"/>
       <c r="V36" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="W36" s="27"/>
       <c r="X36" s="39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Y36" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z36" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="AA36" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="AB36" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC36" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="Z36" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="AA36" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="AB36" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="AC36" s="27" t="s">
+      <c r="AD36" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="AD36" s="21" t="s">
-        <v>260</v>
-      </c>
       <c r="AE36" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF36" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AG36"/>
       <c r="AH36"/>
@@ -5946,7 +5946,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>28</v>
@@ -5975,10 +5975,10 @@
       </c>
       <c r="N37" s="26"/>
       <c r="O37" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P37" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q37" s="27" t="s">
         <v>103</v>
@@ -5988,23 +5988,23 @@
       <c r="T37" s="27"/>
       <c r="U37" s="27"/>
       <c r="V37" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="W37" s="27"/>
       <c r="X37" s="39" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="Y37" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z37" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="AA37" s="21" t="s">
         <v>420</v>
       </c>
-      <c r="AA37" s="21" t="s">
-        <v>421</v>
-      </c>
       <c r="AB37" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AC37" s="27">
         <v>190</v>
@@ -6013,7 +6013,7 @@
         <v>21.1</v>
       </c>
       <c r="AE37" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF37" s="27">
         <v>21.1</v>
@@ -6072,7 +6072,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>25</v>
@@ -6101,36 +6101,36 @@
       </c>
       <c r="N38" s="26"/>
       <c r="O38" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P38" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q38" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R38" s="27"/>
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
       <c r="U38" s="27"/>
       <c r="V38" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W38" s="27"/>
       <c r="X38" s="39" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="Y38" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z38" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="AA38" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="AA38" s="21" t="s">
-        <v>408</v>
-      </c>
       <c r="AB38" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AC38" s="27">
         <v>148</v>
@@ -6139,7 +6139,7 @@
         <v>9.5</v>
       </c>
       <c r="AE38" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF38" s="27">
         <v>22.3</v>
@@ -6198,7 +6198,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>1</v>
@@ -6227,30 +6227,30 @@
         <v>551236001638</v>
       </c>
       <c r="O39" s="27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P39" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q39" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R39" s="27"/>
       <c r="S39" s="27"/>
       <c r="T39" s="27"/>
       <c r="U39" s="27"/>
       <c r="V39" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W39" s="27"/>
       <c r="X39" s="39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Y39" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z39" s="21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AA39" s="21"/>
       <c r="AB39" s="27" t="s">
@@ -6263,7 +6263,7 @@
         <v>52.4</v>
       </c>
       <c r="AE39" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF39" s="27"/>
       <c r="AG39"/>
@@ -6353,10 +6353,10 @@
       <c r="M40" s="47"/>
       <c r="N40" s="26"/>
       <c r="O40" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P40" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q40" s="27" t="s">
         <v>103</v>
@@ -6366,23 +6366,23 @@
       <c r="T40" s="27"/>
       <c r="U40" s="27"/>
       <c r="V40" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W40" s="27"/>
       <c r="X40" s="39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Y40" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z40" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="AA40" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="AB40" s="27" t="s">
         <v>271</v>
-      </c>
-      <c r="Z40" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="AA40" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="AB40" s="27" t="s">
-        <v>272</v>
       </c>
       <c r="AC40" s="27">
         <v>1255</v>
@@ -6391,7 +6391,7 @@
         <v>54.4</v>
       </c>
       <c r="AE40" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF40" s="27">
         <v>83.4</v>
@@ -6450,7 +6450,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>28</v>
@@ -6480,29 +6480,29 @@
       <c r="N41" s="26"/>
       <c r="O41" s="27"/>
       <c r="P41" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q41" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R41" s="27"/>
       <c r="S41" s="27"/>
       <c r="T41" s="27"/>
       <c r="U41" s="27"/>
       <c r="V41" s="27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="W41" s="27"/>
       <c r="X41" s="39" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Y41" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Z41" s="21"/>
       <c r="AA41" s="21"/>
       <c r="AB41" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC41" s="27" t="s">
         <v>113</v>
@@ -6511,7 +6511,7 @@
         <v>113</v>
       </c>
       <c r="AE41" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF41" s="27" t="s">
         <v>113</v>
@@ -6599,34 +6599,34 @@
       <c r="M42" s="25"/>
       <c r="N42" s="26"/>
       <c r="O42" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P42" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q42" s="27" t="s">
         <v>277</v>
-      </c>
-      <c r="Q42" s="27" t="s">
-        <v>278</v>
       </c>
       <c r="R42" s="27"/>
       <c r="S42" s="27"/>
       <c r="T42" s="27"/>
       <c r="U42" s="27"/>
       <c r="V42" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="W42" s="27"/>
       <c r="X42" s="39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Y42" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Z42" s="21" t="s">
         <v>113</v>
       </c>
       <c r="AA42" s="21"/>
       <c r="AB42" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC42" s="27" t="s">
         <v>113</v>
@@ -6635,7 +6635,7 @@
         <v>113</v>
       </c>
       <c r="AE42" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF42" s="27" t="s">
         <v>113</v>
@@ -6694,7 +6694,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C43" s="22">
         <v>6</v>
@@ -6723,30 +6723,30 @@
         <v>551236001639</v>
       </c>
       <c r="O43" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P43" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q43" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R43" s="27"/>
       <c r="S43" s="27"/>
       <c r="T43" s="27"/>
       <c r="U43" s="27"/>
       <c r="V43" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="W43" s="27"/>
       <c r="X43" s="39" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="Y43" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z43" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AA43" s="21"/>
       <c r="AB43" s="27" t="s">
@@ -6759,7 +6759,7 @@
         <v>71</v>
       </c>
       <c r="AE43" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF43" s="27"/>
       <c r="AG43"/>
@@ -6816,7 +6816,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>1</v>
@@ -6841,34 +6841,34 @@
       <c r="M44" s="25"/>
       <c r="N44" s="26"/>
       <c r="O44" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="P44" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q44" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R44" s="27"/>
       <c r="S44" s="27"/>
       <c r="T44" s="27"/>
       <c r="U44" s="27"/>
       <c r="V44" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="W44" s="27"/>
       <c r="X44" s="39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y44" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z44" s="21" t="s">
         <v>114</v>
       </c>
       <c r="AA44" s="21"/>
       <c r="AB44" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC44" s="27">
         <v>624</v>
@@ -6877,7 +6877,7 @@
         <v>113</v>
       </c>
       <c r="AE44" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF44" s="27" t="s">
         <v>113</v>
@@ -6936,7 +6936,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C45" s="22">
         <v>6</v>
@@ -6967,30 +6967,30 @@
         <v>551236002471</v>
       </c>
       <c r="O45" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P45" s="27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q45" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R45" s="27"/>
       <c r="S45" s="27"/>
       <c r="T45" s="27"/>
       <c r="U45" s="27"/>
       <c r="V45" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="W45" s="27"/>
       <c r="X45" s="39" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Y45" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Z45" s="21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AA45" s="21"/>
       <c r="AB45" s="27" t="s">
@@ -7003,7 +7003,7 @@
         <v>42.1</v>
       </c>
       <c r="AE45" s="27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AF45" s="27"/>
       <c r="AG45"/>
@@ -7057,7 +7057,7 @@
     <row r="46" spans="1:79" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A46" s="44"/>
       <c r="B46" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>1</v>
@@ -7091,29 +7091,29 @@
       <c r="N46" s="26"/>
       <c r="O46" s="27"/>
       <c r="P46" s="27" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q46" s="27" t="s">
         <v>475</v>
-      </c>
-      <c r="Q46" s="27" t="s">
-        <v>476</v>
       </c>
       <c r="R46" s="27"/>
       <c r="S46" s="27"/>
       <c r="T46" s="27"/>
       <c r="U46" s="27"/>
       <c r="V46" s="27" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="W46" s="27"/>
       <c r="X46" s="39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Y46" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="Z46" s="21"/>
       <c r="AA46" s="21"/>
       <c r="AB46" s="27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AC46" s="27">
         <v>93</v>
@@ -7122,7 +7122,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="AE46" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AF46" s="27">
         <v>48.9</v>
@@ -7181,7 +7181,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>1</v>
@@ -7214,36 +7214,36 @@
       </c>
       <c r="N47" s="26"/>
       <c r="O47" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P47" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q47" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R47" s="27"/>
       <c r="S47" s="27"/>
       <c r="T47" s="27"/>
       <c r="U47" s="27"/>
       <c r="V47" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="W47" s="27"/>
       <c r="X47" s="39" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y47" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z47" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA47" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="AB47" s="27" t="s">
         <v>291</v>
-      </c>
-      <c r="Z47" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="AA47" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="AB47" s="27" t="s">
-        <v>292</v>
       </c>
       <c r="AC47" s="27">
         <v>187</v>
@@ -7252,7 +7252,7 @@
         <v>41.7</v>
       </c>
       <c r="AE47" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF47" s="27">
         <v>76</v>
@@ -7311,7 +7311,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>1</v>
@@ -7340,10 +7340,10 @@
         <v>551236001614</v>
       </c>
       <c r="O48" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P48" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q48" s="27" t="s">
         <v>85</v>
@@ -7353,17 +7353,17 @@
       <c r="T48" s="27"/>
       <c r="U48" s="27"/>
       <c r="V48" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W48" s="27"/>
       <c r="X48" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y48" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="Y48" s="27" t="s">
-        <v>136</v>
-      </c>
       <c r="Z48" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AA48" s="21"/>
       <c r="AB48" s="27" t="s">
@@ -7376,7 +7376,7 @@
         <v>83.6</v>
       </c>
       <c r="AE48" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF48" s="27"/>
       <c r="AG48"/>
@@ -7433,7 +7433,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>1</v>
@@ -7462,10 +7462,10 @@
         <v>551236001642</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="P49" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q49" s="27" t="s">
         <v>98</v>
@@ -7475,17 +7475,17 @@
       <c r="T49" s="27"/>
       <c r="U49" s="27"/>
       <c r="V49" s="27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W49" s="27"/>
       <c r="X49" s="39" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y49" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Z49" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AA49" s="21"/>
       <c r="AB49" s="27" t="s">
@@ -7498,7 +7498,7 @@
         <v>84.8</v>
       </c>
       <c r="AE49" s="27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF49" s="27"/>
       <c r="AG49"/>
@@ -7555,7 +7555,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C50" s="22">
         <v>6</v>
@@ -7586,30 +7586,30 @@
         <v>551236001644</v>
       </c>
       <c r="O50" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P50" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Q50" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R50" s="27"/>
       <c r="S50" s="27"/>
       <c r="T50" s="27"/>
       <c r="U50" s="27"/>
       <c r="V50" s="27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W50" s="27"/>
       <c r="X50" s="39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Y50" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z50" s="21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AA50" s="21"/>
       <c r="AB50" s="27" t="s">
@@ -7677,7 +7677,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>1</v>
@@ -7706,10 +7706,10 @@
         <v>551236001646</v>
       </c>
       <c r="O51" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P51" s="27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q51" s="27" t="s">
         <v>85</v>
@@ -7719,17 +7719,17 @@
       <c r="T51" s="27"/>
       <c r="U51" s="27"/>
       <c r="V51" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="W51" s="27"/>
       <c r="X51" s="39" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Y51" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Z51" s="21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AA51" s="21"/>
       <c r="AB51" s="27" t="s">
@@ -7742,7 +7742,7 @@
         <v>77.8</v>
       </c>
       <c r="AE51" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF51" s="27"/>
       <c r="AG51"/>
@@ -7832,36 +7832,36 @@
       </c>
       <c r="N52" s="26"/>
       <c r="O52" s="27" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P52" s="27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q52" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R52" s="27"/>
       <c r="S52" s="27"/>
       <c r="T52" s="27"/>
       <c r="U52" s="27"/>
       <c r="V52" s="27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="W52" s="27"/>
       <c r="X52" s="39" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Y52" s="27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Z52" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="AA52" s="21" t="s">
         <v>422</v>
       </c>
-      <c r="AA52" s="21" t="s">
-        <v>423</v>
-      </c>
       <c r="AB52" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AC52" s="27">
         <v>169</v>
@@ -7870,7 +7870,7 @@
         <v>37.299999999999997</v>
       </c>
       <c r="AE52" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF52" s="27">
         <v>81.7</v>

</xml_diff>

<commit_message>
add concordia report cards
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF7E03-E926-B948-A74E-35E5F64184C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7B1693-6555-234B-ACD2-9E1516FAEBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="494">
   <si>
     <t>name</t>
   </si>
@@ -1518,6 +1518,12 @@
   </si>
   <si>
     <t>Kindergarten readiness, special education, Dual-language, Parent-Child Oriented Classroom (P-COC)</t>
+  </si>
+  <si>
+    <t>Concordia_2018-19ALL.PDF</t>
+  </si>
+  <si>
+    <t>Concordia_2018-19CHOICE.PDF</t>
   </si>
 </sst>
 </file>
@@ -2621,10 +2627,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="AE3" sqref="AE3"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3001,7 +3007,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="23">
@@ -3037,8 +3043,12 @@
       <c r="Y5" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
+      <c r="Z5" s="21" t="s">
+        <v>492</v>
+      </c>
+      <c r="AA5" s="21" t="s">
+        <v>493</v>
+      </c>
       <c r="AB5" s="27" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
add report cards for st johns
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E18DC88-1D0F-C84C-8557-06A792DBD42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F8A83-82A4-B040-9B44-B387E1F7056F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1400" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All schools" sheetId="13" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="496">
   <si>
     <t>name</t>
   </si>
@@ -1524,6 +1524,12 @@
   </si>
   <si>
     <t>EverGreen_Academy_2018-19CHOICE.PDF</t>
+  </si>
+  <si>
+    <t>Saint_Johns_2018-19ALL.PDF</t>
+  </si>
+  <si>
+    <t>Saint_Johns_2018-19CHOICE.PDF</t>
   </si>
 </sst>
 </file>
@@ -2627,10 +2633,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5758,8 +5764,12 @@
       <c r="Y35" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="Z35" s="21"/>
-      <c r="AA35" s="21"/>
+      <c r="Z35" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="AA35" s="21" t="s">
+        <v>495</v>
+      </c>
       <c r="AB35" s="27" t="s">
         <v>254</v>
       </c>

</xml_diff>

<commit_message>
add trinity logos and fix name
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F8A83-82A4-B040-9B44-B387E1F7056F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F37324-62C9-E34E-BCCD-4D8E5F9A0B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1400" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="498">
   <si>
     <t>name</t>
   </si>
@@ -1530,6 +1530,12 @@
   </si>
   <si>
     <t>Saint_Johns_2018-19CHOICE.PDF</t>
+  </si>
+  <si>
+    <t>SmallWorld.png</t>
+  </si>
+  <si>
+    <t>TrinityEvangelical.png</t>
   </si>
 </sst>
 </file>
@@ -2633,10 +2639,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="Z35" sqref="Z35"/>
+      <selection pane="bottomLeft" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6497,7 +6503,9 @@
         <v>76</v>
       </c>
       <c r="N41" s="26"/>
-      <c r="O41" s="27"/>
+      <c r="O41" s="27" t="s">
+        <v>496</v>
+      </c>
       <c r="P41" s="27" t="s">
         <v>272</v>
       </c>
@@ -7108,7 +7116,9 @@
         <v>1512619</v>
       </c>
       <c r="N46" s="26"/>
-      <c r="O46" s="27"/>
+      <c r="O46" s="27" t="s">
+        <v>497</v>
+      </c>
       <c r="P46" s="27" t="s">
         <v>473</v>
       </c>

</xml_diff>

<commit_message>
handle historical school id changes/merges
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F37324-62C9-E34E-BCCD-4D8E5F9A0B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C6841D-FD2D-7A49-98E8-C8DB4822EFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1400" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="505">
   <si>
     <t>name</t>
   </si>
@@ -1536,6 +1536,27 @@
   </si>
   <si>
     <t>TrinityEvangelical.png</t>
+  </si>
+  <si>
+    <t>NCES History</t>
+  </si>
+  <si>
+    <t>School Code History</t>
+  </si>
+  <si>
+    <t>2017:551236001625</t>
+  </si>
+  <si>
+    <t>2017:0282</t>
+  </si>
+  <si>
+    <t>2017:0286</t>
+  </si>
+  <si>
+    <t>2017:551236001633</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -2099,7 +2120,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2259,6 +2280,9 @@
     <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2305,7 +2329,35 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2639,10 +2691,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="O46" sqref="O46"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2672,10 +2724,14 @@
     <col min="30" max="30" width="15.1640625" customWidth="1"/>
     <col min="31" max="31" width="17.5" style="9" customWidth="1"/>
     <col min="32" max="32" width="15" style="9" customWidth="1"/>
+    <col min="33" max="33" width="18" customWidth="1"/>
+    <col min="34" max="34" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="13"/>
+    <row r="1" spans="1:34" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>504</v>
+      </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2769,8 +2825,14 @@
       <c r="AF1" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" ht="128" x14ac:dyDescent="0.2">
+      <c r="AG1" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2846,7 +2908,7 @@
       </c>
       <c r="AF2" s="27"/>
     </row>
-    <row r="3" spans="1:32" ht="160" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="160" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <f t="shared" ref="A3:A45" si="0">A2+1</f>
         <v>2</v>
@@ -2919,7 +2981,7 @@
       </c>
       <c r="AF3" s="27"/>
     </row>
-    <row r="4" spans="1:32" ht="144" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2994,7 +3056,7 @@
       </c>
       <c r="AF4" s="27"/>
     </row>
-    <row r="5" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3077,7 +3139,7 @@
         <v>58.8</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3152,7 +3214,7 @@
       </c>
       <c r="AF6" s="27"/>
     </row>
-    <row r="7" spans="1:32" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="44">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3242,7 +3304,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="44">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3317,7 +3379,7 @@
       </c>
       <c r="AF8" s="27"/>
     </row>
-    <row r="9" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="44">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3394,7 +3456,7 @@
       </c>
       <c r="AF9" s="27"/>
     </row>
-    <row r="10" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="44">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3471,7 +3533,7 @@
       </c>
       <c r="AF10" s="27"/>
     </row>
-    <row r="11" spans="1:32" ht="144" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="44">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3554,7 +3616,7 @@
         <v>99.7</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="44">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3629,7 +3691,7 @@
       </c>
       <c r="AF12" s="27"/>
     </row>
-    <row r="13" spans="1:32" ht="96" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="44">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3704,7 +3766,7 @@
       </c>
       <c r="AF13" s="27"/>
     </row>
-    <row r="14" spans="1:32" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="44">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3779,7 +3841,7 @@
       </c>
       <c r="AF14" s="27"/>
     </row>
-    <row r="15" spans="1:32" ht="192" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" ht="192" x14ac:dyDescent="0.2">
       <c r="A15" s="44">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3854,7 +3916,7 @@
       </c>
       <c r="AF15" s="27"/>
     </row>
-    <row r="16" spans="1:32" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="44">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3930,6 +3992,12 @@
         <v>126</v>
       </c>
       <c r="AF16" s="27"/>
+      <c r="AG16" s="27" t="s">
+        <v>500</v>
+      </c>
+      <c r="AH16" s="27" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="17" spans="1:79" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="44">
@@ -4234,6 +4302,12 @@
         <v>196</v>
       </c>
       <c r="AF20" s="27"/>
+      <c r="AG20" s="57" t="s">
+        <v>503</v>
+      </c>
+      <c r="AH20" s="27" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="21" spans="1:79" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="44">
@@ -7082,7 +7156,9 @@
       <c r="CA45"/>
     </row>
     <row r="46" spans="1:79" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
+      <c r="A46" s="44">
+        <v>45</v>
+      </c>
       <c r="B46" s="27" t="s">
         <v>488</v>
       </c>
@@ -7207,7 +7283,7 @@
     <row r="47" spans="1:79" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A47" s="44">
         <f t="shared" ref="A47:A52" si="1">A46+1</f>
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B47" s="27" t="s">
         <v>321</v>
@@ -7337,7 +7413,7 @@
     <row r="48" spans="1:79" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="44">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>312</v>
@@ -7459,7 +7535,7 @@
     <row r="49" spans="1:79" s="2" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A49" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B49" s="27" t="s">
         <v>322</v>
@@ -7581,7 +7657,7 @@
     <row r="50" spans="1:79" s="2" customFormat="1" ht="256" x14ac:dyDescent="0.2">
       <c r="A50" s="44">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B50" s="27" t="s">
         <v>311</v>
@@ -7703,7 +7779,7 @@
     <row r="51" spans="1:79" s="2" customFormat="1" ht="224" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B51" s="27" t="s">
         <v>326</v>
@@ -7825,7 +7901,7 @@
     <row r="52" spans="1:79" s="2" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B52" s="27" t="s">
         <v>12</v>
@@ -8057,23 +8133,67 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF52">
     <sortCondition ref="B2:B52"/>
   </sortState>
-  <conditionalFormatting sqref="A53:AF53 B28:W29 Y28:AF29 A8:A52 B8:AF15 B17:K17 B16:L16 M17 O17:AF17 N16:AF16 B25:AF27 B24:J24 O24:AF24 B18:AF23 B30:AF52 A1:AF6 A7:Y7 AA7:AF7">
+  <conditionalFormatting sqref="A53:AF53 B28:W29 Y28:AF29 A8:A52 B8:AF15 B17:K17 B16:L16 M17 O17:AF17 N16:AF16 B25:AF27 B24:J24 O24:AF24 B18:AF23 B30:AF52 A7:Y7 AA7:AF7 A1:AF6">
+    <cfRule type="expression" dxfId="6" priority="19">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="21">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="22">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="expression" dxfId="5" priority="20">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24:N24">
+    <cfRule type="expression" dxfId="4" priority="13">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="14">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="15">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG1">
+    <cfRule type="expression" dxfId="3" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="11">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="12">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH1">
     <cfRule type="expression" dxfId="2" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="9">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" priority="10">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG16:AH16">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="5">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="6">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24:N24">
+  <conditionalFormatting sqref="AG20:AH20">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add trinity lutheran report card
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C6841D-FD2D-7A49-98E8-C8DB4822EFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6592F27-1C8A-144A-BEE2-9823CC7580F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1400" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="506">
   <si>
     <t>name</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Trinity_Lutheran_2018-19CHOICE.PDF</t>
   </si>
 </sst>
 </file>
@@ -2691,10 +2694,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <selection pane="bottomLeft" activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7216,7 +7219,9 @@
         <v>476</v>
       </c>
       <c r="Z46" s="21"/>
-      <c r="AA46" s="21"/>
+      <c r="AA46" s="21" t="s">
+        <v>505</v>
+      </c>
       <c r="AB46" s="27" t="s">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
update st cats numstudents
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F6C00-8977-0F42-9FD0-AAB86B083F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7A0E94-2A80-2C47-A135-FBC0C5A2A475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1400" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,9 +786,6 @@
     <t>St. Catherine’s educates students in the Catholic faith, fostering an environment of academic and behavioral excellence to create lifelong learners and globally responsible citizens. St. Catherine’s is built on the Dominican values of Study, Prayer, Service and Community.</t>
   </si>
   <si>
-    <t>687*</t>
-  </si>
-  <si>
     <t>100*</t>
   </si>
   <si>
@@ -1566,6 +1563,9 @@
   </si>
   <si>
     <t>Academic, Right of Passage Experience (ROPE) for high school students</t>
+  </si>
+  <si>
+    <t>667*</t>
   </si>
 </sst>
 </file>
@@ -2700,10 +2700,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="AE50" sqref="AE50"/>
+      <selection pane="bottomLeft" activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2739,7 +2739,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -2763,7 +2763,7 @@
         <v>60</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>61</v>
@@ -2793,22 +2793,22 @@
         <v>83</v>
       </c>
       <c r="S1" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="V1" s="19" t="s">
         <v>457</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>454</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="V1" s="19" t="s">
-        <v>458</v>
       </c>
       <c r="W1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Y1" s="38" t="s">
         <v>78</v>
@@ -2838,10 +2838,10 @@
         <v>96</v>
       </c>
       <c r="AH1" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="AI1" s="19" t="s">
         <v>498</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="128" x14ac:dyDescent="0.2">
@@ -2881,7 +2881,7 @@
         <v>550004502575</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q2" s="28" t="s">
         <v>97</v>
@@ -2904,7 +2904,7 @@
         <v>101</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AB2" s="21"/>
       <c r="AC2" s="27" t="s">
@@ -2957,7 +2957,7 @@
         <v>551236002708</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q3" s="27" t="s">
         <v>102</v>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="X3" s="27"/>
       <c r="Y3" s="39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Z3" s="27" t="s">
         <v>105</v>
@@ -2991,7 +2991,7 @@
         <v>114</v>
       </c>
       <c r="AF3" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AG3" s="27"/>
     </row>
@@ -3031,7 +3031,7 @@
       <c r="N4" s="25"/>
       <c r="O4" s="26"/>
       <c r="P4" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q4" s="27" t="s">
         <v>106</v>
@@ -3054,7 +3054,7 @@
         <v>109</v>
       </c>
       <c r="AA4" s="54" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AB4" s="21"/>
       <c r="AC4" s="27" t="s">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="O5" s="26"/>
       <c r="P5" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q5" s="27" t="s">
         <v>117</v>
@@ -3124,7 +3124,7 @@
       <c r="U5" s="27"/>
       <c r="V5" s="27"/>
       <c r="W5" s="27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="X5" s="27"/>
       <c r="Y5" s="39" t="s">
@@ -3134,10 +3134,10 @@
         <v>120</v>
       </c>
       <c r="AA5" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="AB5" s="21" t="s">
         <v>491</v>
-      </c>
-      <c r="AB5" s="21" t="s">
-        <v>492</v>
       </c>
       <c r="AC5" s="27" t="s">
         <v>121</v>
@@ -3161,7 +3161,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>1</v>
@@ -3191,7 +3191,7 @@
         <v>551236001627</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q6" s="27" t="s">
         <v>179</v>
@@ -3214,7 +3214,7 @@
         <v>182</v>
       </c>
       <c r="AA6" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AB6" s="21"/>
       <c r="AC6" s="27" t="s">
@@ -3271,25 +3271,25 @@
       </c>
       <c r="O7" s="26"/>
       <c r="P7" s="27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Q7" s="27" t="s">
+        <v>461</v>
+      </c>
+      <c r="R7" s="27" t="s">
+        <v>463</v>
+      </c>
+      <c r="S7" s="27" t="s">
+        <v>458</v>
+      </c>
+      <c r="T7" s="27" t="s">
+        <v>460</v>
+      </c>
+      <c r="U7" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="R7" s="27" t="s">
-        <v>464</v>
-      </c>
-      <c r="S7" s="27" t="s">
+      <c r="V7" s="27" t="s">
         <v>459</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>461</v>
-      </c>
-      <c r="U7" s="27" t="s">
-        <v>463</v>
-      </c>
-      <c r="V7" s="27" t="s">
-        <v>460</v>
       </c>
       <c r="W7" s="27" t="s">
         <v>123</v>
@@ -3298,13 +3298,13 @@
         <v>123</v>
       </c>
       <c r="Y7" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Z7" s="27" t="s">
         <v>124</v>
       </c>
       <c r="AB7" s="21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AC7" s="27" t="s">
         <v>125</v>
@@ -3358,7 +3358,7 @@
         <v>551236001611</v>
       </c>
       <c r="P8" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q8" s="27" t="s">
         <v>127</v>
@@ -3381,7 +3381,7 @@
         <v>131</v>
       </c>
       <c r="AA8" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AB8" s="21"/>
       <c r="AC8" s="27" t="s">
@@ -3404,7 +3404,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>1</v>
@@ -3436,7 +3436,7 @@
         <v>551236002311</v>
       </c>
       <c r="P9" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q9" s="27" t="s">
         <v>136</v>
@@ -3459,7 +3459,7 @@
         <v>139</v>
       </c>
       <c r="AA9" s="21" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AB9" s="21"/>
       <c r="AC9" s="27" t="s">
@@ -3482,7 +3482,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>25</v>
@@ -3516,7 +3516,7 @@
         <v>551236001608</v>
       </c>
       <c r="P10" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q10" s="27" t="s">
         <v>140</v>
@@ -3539,7 +3539,7 @@
         <v>143</v>
       </c>
       <c r="AA10" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AB10" s="21"/>
       <c r="AC10" s="27" t="s">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="O11" s="26"/>
       <c r="P11" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q11" s="27" t="s">
         <v>145</v>
@@ -3619,10 +3619,10 @@
         <v>149</v>
       </c>
       <c r="AA11" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="AB11" s="21" t="s">
         <v>378</v>
-      </c>
-      <c r="AB11" s="21" t="s">
-        <v>379</v>
       </c>
       <c r="AC11" s="27" t="s">
         <v>150</v>
@@ -3676,7 +3676,7 @@
         <v>551236001620</v>
       </c>
       <c r="P12" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q12" s="27" t="s">
         <v>151</v>
@@ -3699,7 +3699,7 @@
         <v>154</v>
       </c>
       <c r="AA12" s="21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AB12" s="21"/>
       <c r="AC12" s="27" t="s">
@@ -3752,7 +3752,7 @@
         <v>551236001621</v>
       </c>
       <c r="P13" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q13" s="28" t="s">
         <v>84</v>
@@ -3775,7 +3775,7 @@
         <v>88</v>
       </c>
       <c r="AA13" s="55" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AB13" s="21"/>
       <c r="AC13" s="27" t="s">
@@ -3828,7 +3828,7 @@
         <v>551236001622</v>
       </c>
       <c r="P14" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q14" s="27" t="s">
         <v>156</v>
@@ -3851,7 +3851,7 @@
         <v>159</v>
       </c>
       <c r="AA14" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AB14" s="21"/>
       <c r="AC14" s="27" t="s">
@@ -3874,7 +3874,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>1</v>
@@ -3906,7 +3906,7 @@
         <v>551236001623</v>
       </c>
       <c r="P15" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q15" s="27" t="s">
         <v>161</v>
@@ -3929,7 +3929,7 @@
         <v>164</v>
       </c>
       <c r="AA15" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AB15" s="21"/>
       <c r="AC15" s="27" t="s">
@@ -3952,7 +3952,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>1</v>
@@ -3984,7 +3984,7 @@
         <v>551236001624</v>
       </c>
       <c r="P16" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Q16" s="27" t="s">
         <v>166</v>
@@ -4007,7 +4007,7 @@
         <v>169</v>
       </c>
       <c r="AA16" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AB16" s="21"/>
       <c r="AC16" s="27" t="s">
@@ -4024,10 +4024,10 @@
       </c>
       <c r="AG16" s="27"/>
       <c r="AH16" s="27" t="s">
+        <v>499</v>
+      </c>
+      <c r="AI16" s="27" t="s">
         <v>500</v>
-      </c>
-      <c r="AI16" s="27" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="17" spans="1:80" ht="32" x14ac:dyDescent="0.2">
@@ -4066,7 +4066,7 @@
         <v>1507085</v>
       </c>
       <c r="P17" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q17" s="27" t="s">
         <v>170</v>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="AA17" s="21"/>
       <c r="AB17" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AC17" s="27" t="s">
         <v>174</v>
@@ -4105,7 +4105,7 @@
         <v>122</v>
       </c>
       <c r="AG17" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:80" ht="80" x14ac:dyDescent="0.2">
@@ -4114,7 +4114,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>1</v>
@@ -4144,7 +4144,7 @@
         <v>551236003337</v>
       </c>
       <c r="P18" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Q18" s="27" t="s">
         <v>183</v>
@@ -4167,7 +4167,7 @@
         <v>186</v>
       </c>
       <c r="AA18" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AB18" s="21"/>
       <c r="AC18" s="27" t="s">
@@ -4190,7 +4190,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>1</v>
@@ -4220,7 +4220,7 @@
         <v>551236001628</v>
       </c>
       <c r="P19" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q19" s="27" t="s">
         <v>188</v>
@@ -4243,7 +4243,7 @@
         <v>191</v>
       </c>
       <c r="AA19" s="21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AB19" s="21"/>
       <c r="AC19" s="27" t="s">
@@ -4298,7 +4298,7 @@
         <v>551236001632</v>
       </c>
       <c r="P20" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q20" s="27" t="s">
         <v>192</v>
@@ -4321,7 +4321,7 @@
         <v>195</v>
       </c>
       <c r="AA20" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AB20" s="21"/>
       <c r="AC20" s="27" t="s">
@@ -4338,10 +4338,10 @@
       </c>
       <c r="AG20" s="27"/>
       <c r="AH20" s="57" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AI20" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:80" ht="112" x14ac:dyDescent="0.2">
@@ -4380,7 +4380,7 @@
         <v>551236001634</v>
       </c>
       <c r="P21" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q21" s="27" t="s">
         <v>197</v>
@@ -4403,7 +4403,7 @@
         <v>200</v>
       </c>
       <c r="AA21" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AB21" s="21"/>
       <c r="AC21" s="27" t="s">
@@ -4456,7 +4456,7 @@
         <v>551236001605</v>
       </c>
       <c r="P22" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q22" s="27" t="s">
         <v>201</v>
@@ -4479,7 +4479,7 @@
         <v>204</v>
       </c>
       <c r="AA22" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AB22" s="21"/>
       <c r="AC22" s="27" t="s">
@@ -4534,7 +4534,7 @@
       </c>
       <c r="O23" s="26"/>
       <c r="P23" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q23" s="27" t="s">
         <v>205</v>
@@ -4551,14 +4551,14 @@
       </c>
       <c r="X23" s="27"/>
       <c r="Y23" s="51" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Z23" s="27" t="s">
         <v>207</v>
       </c>
       <c r="AA23" s="21"/>
       <c r="AB23" s="21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AC23" s="27" t="s">
         <v>174</v>
@@ -4612,7 +4612,7 @@
         <v>551236001635</v>
       </c>
       <c r="P24" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q24" s="27" t="s">
         <v>209</v>
@@ -4629,13 +4629,13 @@
       </c>
       <c r="X24" s="27"/>
       <c r="Y24" s="39" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="Z24" s="27" t="s">
         <v>211</v>
       </c>
       <c r="AA24" s="21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AB24" s="21"/>
       <c r="AC24" s="27" t="s">
@@ -4692,7 +4692,7 @@
         <v>551236003045</v>
       </c>
       <c r="P25" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q25" s="27" t="s">
         <v>218</v>
@@ -4709,13 +4709,13 @@
       </c>
       <c r="X25" s="46"/>
       <c r="Y25" s="43" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Z25" s="27" t="s">
         <v>220</v>
       </c>
       <c r="AA25" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AB25" s="21"/>
       <c r="AC25" s="27" t="s">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="O26" s="35"/>
       <c r="P26" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Q26" s="36" t="s">
         <v>222</v>
@@ -4789,14 +4789,14 @@
       </c>
       <c r="X26" s="36"/>
       <c r="Y26" s="53" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z26" s="36" t="s">
         <v>224</v>
       </c>
       <c r="AA26" s="30"/>
       <c r="AB26" s="30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AC26" s="36" t="s">
         <v>225</v>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="O27" s="26"/>
       <c r="P27" s="27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q27" s="27" t="s">
         <v>226</v>
@@ -4869,16 +4869,16 @@
       </c>
       <c r="X27" s="27"/>
       <c r="Y27" s="39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Z27" s="27" t="s">
         <v>228</v>
       </c>
       <c r="AA27" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="AB27" s="21" t="s">
         <v>389</v>
-      </c>
-      <c r="AB27" s="21" t="s">
-        <v>390</v>
       </c>
       <c r="AC27" s="27" t="s">
         <v>229</v>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="O28" s="26"/>
       <c r="P28" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q28" s="27" t="s">
         <v>230</v>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="X28" s="46"/>
       <c r="Y28" s="52" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Z28" s="27" t="s">
         <v>232</v>
@@ -5078,7 +5078,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>1</v>
@@ -5110,7 +5110,7 @@
         <v>551236001636</v>
       </c>
       <c r="P29" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q29" s="27" t="s">
         <v>234</v>
@@ -5127,13 +5127,13 @@
       </c>
       <c r="X29" s="46"/>
       <c r="Y29" s="52" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Z29" s="27" t="s">
         <v>236</v>
       </c>
       <c r="AA29" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AB29" s="21"/>
       <c r="AC29" s="27" t="s">
@@ -5146,7 +5146,7 @@
         <v>52.1</v>
       </c>
       <c r="AF29" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AG29" s="27"/>
       <c r="AH29"/>
@@ -5233,47 +5233,47 @@
         <v>1619</v>
       </c>
       <c r="N30" s="25" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O30" s="26"/>
       <c r="P30" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q30" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="R30" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="S30" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="T30" s="27" t="s">
         <v>468</v>
-      </c>
-      <c r="R30" s="27" t="s">
-        <v>470</v>
-      </c>
-      <c r="S30" s="27" t="s">
-        <v>466</v>
-      </c>
-      <c r="T30" s="27" t="s">
-        <v>469</v>
       </c>
       <c r="U30" s="27" t="s">
         <v>103</v>
       </c>
       <c r="V30" s="27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="W30" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="X30" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="X30" s="27" t="s">
-        <v>472</v>
-      </c>
       <c r="Y30" s="45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Z30" s="27" t="s">
         <v>237</v>
       </c>
       <c r="AA30" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="AB30" s="21" t="s">
         <v>400</v>
-      </c>
-      <c r="AB30" s="21" t="s">
-        <v>401</v>
       </c>
       <c r="AC30" s="27" t="s">
         <v>238</v>
@@ -5344,7 +5344,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>1</v>
@@ -5374,7 +5374,7 @@
         <v>551236001637</v>
       </c>
       <c r="P31" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q31" s="27" t="s">
         <v>239</v>
@@ -5391,13 +5391,13 @@
       </c>
       <c r="X31" s="27"/>
       <c r="Y31" s="39" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Z31" s="27" t="s">
         <v>241</v>
       </c>
       <c r="AA31" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AB31" s="21"/>
       <c r="AC31" s="27" t="s">
@@ -5467,7 +5467,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>1</v>
@@ -5499,7 +5499,7 @@
         <v>551236003044</v>
       </c>
       <c r="P32" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Q32" s="27" t="s">
         <v>242</v>
@@ -5516,13 +5516,13 @@
       </c>
       <c r="X32" s="27"/>
       <c r="Y32" s="39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Z32" s="27" t="s">
         <v>245</v>
       </c>
       <c r="AA32" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AB32" s="21"/>
       <c r="AC32" s="27" t="s">
@@ -5592,7 +5592,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>1</v>
@@ -5622,7 +5622,7 @@
         <v>551236001626</v>
       </c>
       <c r="P33" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q33" s="27" t="s">
         <v>175</v>
@@ -5645,7 +5645,7 @@
         <v>178</v>
       </c>
       <c r="AA33" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AB33" s="21"/>
       <c r="AC33" s="27" t="s">
@@ -5745,7 +5745,7 @@
       </c>
       <c r="O34" s="26"/>
       <c r="P34" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Q34" s="27" t="s">
         <v>246</v>
@@ -5762,22 +5762,22 @@
       </c>
       <c r="X34" s="27"/>
       <c r="Y34" s="39" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Z34" s="27" t="s">
         <v>248</v>
       </c>
       <c r="AA34" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="AB34" s="21" t="s">
         <v>416</v>
-      </c>
-      <c r="AB34" s="21" t="s">
-        <v>417</v>
       </c>
       <c r="AC34" s="27" t="s">
         <v>174</v>
       </c>
       <c r="AD34" s="27" t="s">
-        <v>249</v>
+        <v>507</v>
       </c>
       <c r="AE34" s="21">
         <v>51.9</v>
@@ -5786,7 +5786,7 @@
         <v>122</v>
       </c>
       <c r="AG34" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AH34"/>
       <c r="AI34"/>
@@ -5876,10 +5876,10 @@
       </c>
       <c r="O35" s="26"/>
       <c r="P35" s="27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Q35" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="R35" s="27" t="s">
         <v>146</v>
@@ -5889,23 +5889,23 @@
       <c r="U35" s="27"/>
       <c r="V35" s="27"/>
       <c r="W35" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="X35" s="27"/>
       <c r="Y35" s="39" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Z35" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA35" s="21" t="s">
+        <v>493</v>
+      </c>
+      <c r="AB35" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="AC35" s="27" t="s">
         <v>253</v>
-      </c>
-      <c r="AA35" s="21" t="s">
-        <v>494</v>
-      </c>
-      <c r="AB35" s="21" t="s">
-        <v>495</v>
-      </c>
-      <c r="AC35" s="27" t="s">
-        <v>254</v>
       </c>
       <c r="AD35" s="27">
         <v>222</v>
@@ -6003,10 +6003,10 @@
       <c r="N36" s="25"/>
       <c r="O36" s="26"/>
       <c r="P36" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Q36" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R36" s="27" t="s">
         <v>146</v>
@@ -6016,35 +6016,35 @@
       <c r="U36" s="27"/>
       <c r="V36" s="27"/>
       <c r="W36" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="X36" s="27"/>
       <c r="Y36" s="39" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Z36" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AA36" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="AB36" s="21" t="s">
         <v>403</v>
-      </c>
-      <c r="AB36" s="21" t="s">
-        <v>404</v>
       </c>
       <c r="AC36" s="27" t="s">
         <v>174</v>
       </c>
       <c r="AD36" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="AE36" s="21" t="s">
         <v>258</v>
-      </c>
-      <c r="AE36" s="21" t="s">
-        <v>259</v>
       </c>
       <c r="AF36" s="27" t="s">
         <v>122</v>
       </c>
       <c r="AG36" s="27" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AH36"/>
       <c r="AI36"/>
@@ -6100,7 +6100,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>28</v>
@@ -6130,10 +6130,10 @@
       </c>
       <c r="O37" s="26"/>
       <c r="P37" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="Q37" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R37" s="27" t="s">
         <v>103</v>
@@ -6143,20 +6143,20 @@
       <c r="U37" s="27"/>
       <c r="V37" s="27"/>
       <c r="W37" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="X37" s="27"/>
       <c r="Y37" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Z37" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA37" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="AB37" s="21" t="s">
         <v>418</v>
-      </c>
-      <c r="AB37" s="21" t="s">
-        <v>419</v>
       </c>
       <c r="AC37" s="27" t="s">
         <v>174</v>
@@ -6227,7 +6227,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>25</v>
@@ -6257,10 +6257,10 @@
       </c>
       <c r="O38" s="26"/>
       <c r="P38" s="27" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q38" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="R38" s="27" t="s">
         <v>146</v>
@@ -6270,20 +6270,20 @@
       <c r="U38" s="27"/>
       <c r="V38" s="27"/>
       <c r="W38" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X38" s="27"/>
       <c r="Y38" s="39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Z38" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AA38" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB38" s="21" t="s">
         <v>405</v>
-      </c>
-      <c r="AB38" s="21" t="s">
-        <v>406</v>
       </c>
       <c r="AC38" s="27" t="s">
         <v>174</v>
@@ -6354,7 +6354,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>1</v>
@@ -6384,10 +6384,10 @@
         <v>551236001638</v>
       </c>
       <c r="P39" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q39" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R39" s="27" t="s">
         <v>118</v>
@@ -6397,17 +6397,17 @@
       <c r="U39" s="27"/>
       <c r="V39" s="27"/>
       <c r="W39" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X39" s="27"/>
       <c r="Y39" s="39" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="Z39" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AA39" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AB39" s="21"/>
       <c r="AC39" s="27" t="s">
@@ -6511,10 +6511,10 @@
       <c r="N40" s="47"/>
       <c r="O40" s="26"/>
       <c r="P40" s="27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="Q40" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="R40" s="27" t="s">
         <v>103</v>
@@ -6524,23 +6524,23 @@
       <c r="U40" s="27"/>
       <c r="V40" s="27"/>
       <c r="W40" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X40" s="27"/>
       <c r="Y40" s="39" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="Z40" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA40" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="AB40" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="AC40" s="27" t="s">
         <v>270</v>
-      </c>
-      <c r="AA40" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="AB40" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="AC40" s="27" t="s">
-        <v>271</v>
       </c>
       <c r="AD40" s="27">
         <v>1255</v>
@@ -6608,7 +6608,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>28</v>
@@ -6638,10 +6638,10 @@
       </c>
       <c r="O41" s="26"/>
       <c r="P41" s="27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q41" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R41" s="27" t="s">
         <v>146</v>
@@ -6651,14 +6651,14 @@
       <c r="U41" s="27"/>
       <c r="V41" s="27"/>
       <c r="W41" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="X41" s="27"/>
       <c r="Y41" s="39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Z41" s="27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AA41" s="21"/>
       <c r="AB41" s="21"/>
@@ -6672,7 +6672,7 @@
         <v>113</v>
       </c>
       <c r="AF41" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AG41" s="27" t="s">
         <v>113</v>
@@ -6761,27 +6761,27 @@
       <c r="N42" s="25"/>
       <c r="O42" s="26"/>
       <c r="P42" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Q42" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="R42" s="27" t="s">
         <v>276</v>
-      </c>
-      <c r="R42" s="27" t="s">
-        <v>277</v>
       </c>
       <c r="S42" s="27"/>
       <c r="T42" s="27"/>
       <c r="U42" s="27"/>
       <c r="V42" s="27"/>
       <c r="W42" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="X42" s="27"/>
       <c r="Y42" s="39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Z42" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AA42" s="21" t="s">
         <v>113</v>
@@ -6856,7 +6856,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C43" s="22">
         <v>6</v>
@@ -6888,10 +6888,10 @@
         <v>551236001639</v>
       </c>
       <c r="P43" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q43" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R43" s="27" t="s">
         <v>128</v>
@@ -6901,17 +6901,17 @@
       <c r="U43" s="27"/>
       <c r="V43" s="27"/>
       <c r="W43" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X43" s="27"/>
       <c r="Y43" s="39" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Z43" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA43" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AB43" s="21"/>
       <c r="AC43" s="27" t="s">
@@ -6924,7 +6924,7 @@
         <v>71</v>
       </c>
       <c r="AF43" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AG43" s="27"/>
       <c r="AH43"/>
@@ -6981,7 +6981,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>1</v>
@@ -7007,7 +7007,7 @@
       <c r="N44" s="25"/>
       <c r="O44" s="26"/>
       <c r="P44" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q44" s="27" t="s">
         <v>215</v>
@@ -7024,7 +7024,7 @@
       </c>
       <c r="X44" s="27"/>
       <c r="Y44" s="39" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Z44" s="27" t="s">
         <v>217</v>
@@ -7102,7 +7102,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C45" s="22">
         <v>6</v>
@@ -7136,10 +7136,10 @@
         <v>551236002471</v>
       </c>
       <c r="P45" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q45" s="27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R45" s="27" t="s">
         <v>118</v>
@@ -7149,17 +7149,17 @@
       <c r="U45" s="27"/>
       <c r="V45" s="27"/>
       <c r="W45" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="X45" s="27"/>
       <c r="Y45" s="39" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Z45" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA45" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AB45" s="21"/>
       <c r="AC45" s="27" t="s">
@@ -7172,7 +7172,7 @@
         <v>42.1</v>
       </c>
       <c r="AF45" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AG45" s="27"/>
       <c r="AH45"/>
@@ -7228,7 +7228,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>1</v>
@@ -7262,34 +7262,34 @@
       </c>
       <c r="O46" s="26"/>
       <c r="P46" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q46" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="R46" s="27" t="s">
         <v>473</v>
-      </c>
-      <c r="R46" s="27" t="s">
-        <v>474</v>
       </c>
       <c r="S46" s="27"/>
       <c r="T46" s="27"/>
       <c r="U46" s="27"/>
       <c r="V46" s="27"/>
       <c r="W46" s="27" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="X46" s="27"/>
       <c r="Y46" s="39" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="Z46" s="27" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AA46" s="21"/>
       <c r="AB46" s="21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="AC46" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AD46" s="27">
         <v>93</v>
@@ -7298,7 +7298,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="AF46" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AG46" s="27">
         <v>48.9</v>
@@ -7357,7 +7357,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>1</v>
@@ -7391,10 +7391,10 @@
       </c>
       <c r="O47" s="26"/>
       <c r="P47" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Q47" s="27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R47" s="27" t="s">
         <v>146</v>
@@ -7404,23 +7404,23 @@
       <c r="U47" s="27"/>
       <c r="V47" s="27"/>
       <c r="W47" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X47" s="27"/>
       <c r="Y47" s="39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Z47" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="AA47" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="AB47" s="21" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC47" s="27" t="s">
         <v>290</v>
-      </c>
-      <c r="AA47" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="AB47" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="AC47" s="27" t="s">
-        <v>291</v>
       </c>
       <c r="AD47" s="27">
         <v>187</v>
@@ -7488,7 +7488,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>1</v>
@@ -7518,7 +7518,7 @@
         <v>551236001614</v>
       </c>
       <c r="P48" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q48" s="27" t="s">
         <v>132</v>
@@ -7541,7 +7541,7 @@
         <v>135</v>
       </c>
       <c r="AA48" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AB48" s="21"/>
       <c r="AC48" s="27" t="s">
@@ -7611,7 +7611,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>1</v>
@@ -7641,10 +7641,10 @@
         <v>551236001642</v>
       </c>
       <c r="P49" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q49" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="R49" s="27" t="s">
         <v>98</v>
@@ -7654,17 +7654,17 @@
       <c r="U49" s="27"/>
       <c r="V49" s="27"/>
       <c r="W49" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="X49" s="27"/>
       <c r="Y49" s="39" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Z49" s="27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA49" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AB49" s="21"/>
       <c r="AC49" s="27" t="s">
@@ -7677,7 +7677,7 @@
         <v>84.8</v>
       </c>
       <c r="AF49" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AG49" s="27"/>
       <c r="AH49"/>
@@ -7734,7 +7734,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C50" s="22">
         <v>6</v>
@@ -7768,10 +7768,10 @@
         <v>551236001644</v>
       </c>
       <c r="P50" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q50" s="27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="R50" s="27" t="s">
         <v>128</v>
@@ -7781,17 +7781,17 @@
       <c r="U50" s="27"/>
       <c r="V50" s="27"/>
       <c r="W50" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="X50" s="27"/>
       <c r="Y50" s="39" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Z50" s="27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AA50" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AB50" s="21"/>
       <c r="AC50" s="27" t="s">
@@ -7804,7 +7804,7 @@
         <v>35.4</v>
       </c>
       <c r="AF50" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AG50" s="27"/>
       <c r="AH50"/>
@@ -7861,7 +7861,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>1</v>
@@ -7891,10 +7891,10 @@
         <v>551236001646</v>
       </c>
       <c r="P51" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q51" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R51" s="27" t="s">
         <v>85</v>
@@ -7904,17 +7904,17 @@
       <c r="U51" s="27"/>
       <c r="V51" s="27"/>
       <c r="W51" s="27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="X51" s="27"/>
       <c r="Y51" s="39" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Z51" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AA51" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AB51" s="21"/>
       <c r="AC51" s="27" t="s">
@@ -7927,7 +7927,7 @@
         <v>77.8</v>
       </c>
       <c r="AF51" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AG51" s="27"/>
       <c r="AH51"/>
@@ -8018,10 +8018,10 @@
       </c>
       <c r="O52" s="26"/>
       <c r="P52" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q52" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R52" s="27" t="s">
         <v>146</v>
@@ -8031,23 +8031,23 @@
       <c r="U52" s="27"/>
       <c r="V52" s="27"/>
       <c r="W52" s="27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X52" s="27"/>
       <c r="Y52" s="39" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="Z52" s="27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA52" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB52" s="21" t="s">
         <v>420</v>
       </c>
-      <c r="AB52" s="21" t="s">
-        <v>421</v>
-      </c>
       <c r="AC52" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AD52" s="27">
         <v>169</v>

</xml_diff>

<commit_message>
fix cert school data
</commit_message>
<xml_diff>
--- a/scripts/data/racine-schools-directory.xlsx
+++ b/scripts/data/racine-schools-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griswold/project/racine-schools/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7A0E94-2A80-2C47-A135-FBC0C5A2A475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE74CC5C-68D0-5343-ACE7-C853D8E46924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1400" windowWidth="26460" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2700,10 +2700,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="AD34" sqref="AD34"/>
+      <selection pane="bottomLeft" activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3053,15 +3053,15 @@
       <c r="Z4" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="AA4" s="54" t="s">
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="AB4" s="21"/>
       <c r="AC4" s="27" t="s">
         <v>115</v>
       </c>
       <c r="AD4" s="27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE4" s="21">
         <v>100</v>
@@ -3069,7 +3069,9 @@
       <c r="AF4" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="AG4" s="27"/>
+      <c r="AG4" s="27">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:35" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="13">

</xml_diff>